<commit_message>
Progress on the interim report
</commit_message>
<xml_diff>
--- a/docs/Proposal and Planning/GANTT.xlsx
+++ b/docs/Proposal and Planning/GANTT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF548C4-C134-4FBD-8ADA-4A5E44AB4B84}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427929E4-EE3C-47C0-9778-8E50F1630ECD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>Create a project schedule in this worksheet.
 Enter the title of this project in cell B1. 
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>Writing the Code Generator</t>
+  </si>
+  <si>
+    <t>Writing Interim</t>
   </si>
 </sst>
 </file>
@@ -1232,6 +1235,9 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="12" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="171" fontId="7" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="169" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1242,9 +1248,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="20% - Accent1" xfId="31" builtinId="30" customBuiltin="1"/>
@@ -1852,11 +1855,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:GU30"/>
+  <dimension ref="A1:GU31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB15" sqref="AB15"/>
+      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA16" sqref="AA16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1899,10 +1902,10 @@
       </c>
       <c r="B3" s="36"/>
       <c r="C3" s="55"/>
-      <c r="D3" s="76">
+      <c r="D3" s="72">
         <v>43738</v>
       </c>
-      <c r="E3" s="76"/>
+      <c r="E3" s="72"/>
     </row>
     <row r="4" spans="1:203" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
@@ -1912,296 +1915,296 @@
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="H4" s="72">
+      <c r="H4" s="73">
         <f>H5</f>
         <v>43738</v>
       </c>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="74"/>
-      <c r="O4" s="72">
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="74"/>
+      <c r="N4" s="75"/>
+      <c r="O4" s="73">
         <f>O5</f>
         <v>43745</v>
       </c>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="73"/>
-      <c r="R4" s="73"/>
-      <c r="S4" s="73"/>
-      <c r="T4" s="73"/>
-      <c r="U4" s="74"/>
-      <c r="V4" s="72">
+      <c r="P4" s="74"/>
+      <c r="Q4" s="74"/>
+      <c r="R4" s="74"/>
+      <c r="S4" s="74"/>
+      <c r="T4" s="74"/>
+      <c r="U4" s="75"/>
+      <c r="V4" s="73">
         <f>V5</f>
         <v>43752</v>
       </c>
-      <c r="W4" s="73"/>
-      <c r="X4" s="73"/>
-      <c r="Y4" s="73"/>
-      <c r="Z4" s="73"/>
-      <c r="AA4" s="73"/>
-      <c r="AB4" s="74"/>
-      <c r="AC4" s="72">
+      <c r="W4" s="74"/>
+      <c r="X4" s="74"/>
+      <c r="Y4" s="74"/>
+      <c r="Z4" s="74"/>
+      <c r="AA4" s="74"/>
+      <c r="AB4" s="75"/>
+      <c r="AC4" s="73">
         <f>AC5</f>
         <v>43759</v>
       </c>
-      <c r="AD4" s="73"/>
-      <c r="AE4" s="73"/>
-      <c r="AF4" s="73"/>
-      <c r="AG4" s="73"/>
-      <c r="AH4" s="73"/>
-      <c r="AI4" s="74"/>
-      <c r="AJ4" s="72">
+      <c r="AD4" s="74"/>
+      <c r="AE4" s="74"/>
+      <c r="AF4" s="74"/>
+      <c r="AG4" s="74"/>
+      <c r="AH4" s="74"/>
+      <c r="AI4" s="75"/>
+      <c r="AJ4" s="73">
         <f>AJ5</f>
         <v>43766</v>
       </c>
-      <c r="AK4" s="73"/>
-      <c r="AL4" s="73"/>
-      <c r="AM4" s="73"/>
-      <c r="AN4" s="73"/>
-      <c r="AO4" s="73"/>
-      <c r="AP4" s="74"/>
-      <c r="AQ4" s="72">
+      <c r="AK4" s="74"/>
+      <c r="AL4" s="74"/>
+      <c r="AM4" s="74"/>
+      <c r="AN4" s="74"/>
+      <c r="AO4" s="74"/>
+      <c r="AP4" s="75"/>
+      <c r="AQ4" s="73">
         <f>AQ5</f>
         <v>43773</v>
       </c>
-      <c r="AR4" s="73"/>
-      <c r="AS4" s="73"/>
-      <c r="AT4" s="73"/>
-      <c r="AU4" s="73"/>
-      <c r="AV4" s="73"/>
-      <c r="AW4" s="74"/>
-      <c r="AX4" s="72">
+      <c r="AR4" s="74"/>
+      <c r="AS4" s="74"/>
+      <c r="AT4" s="74"/>
+      <c r="AU4" s="74"/>
+      <c r="AV4" s="74"/>
+      <c r="AW4" s="75"/>
+      <c r="AX4" s="73">
         <f>AX5</f>
         <v>43780</v>
       </c>
-      <c r="AY4" s="73"/>
-      <c r="AZ4" s="73"/>
-      <c r="BA4" s="73"/>
-      <c r="BB4" s="73"/>
-      <c r="BC4" s="73"/>
-      <c r="BD4" s="74"/>
-      <c r="BE4" s="72">
+      <c r="AY4" s="74"/>
+      <c r="AZ4" s="74"/>
+      <c r="BA4" s="74"/>
+      <c r="BB4" s="74"/>
+      <c r="BC4" s="74"/>
+      <c r="BD4" s="75"/>
+      <c r="BE4" s="73">
         <f>BE5</f>
         <v>43787</v>
       </c>
-      <c r="BF4" s="73"/>
-      <c r="BG4" s="73"/>
-      <c r="BH4" s="73"/>
-      <c r="BI4" s="73"/>
-      <c r="BJ4" s="73"/>
-      <c r="BK4" s="74"/>
-      <c r="BL4" s="72">
+      <c r="BF4" s="74"/>
+      <c r="BG4" s="74"/>
+      <c r="BH4" s="74"/>
+      <c r="BI4" s="74"/>
+      <c r="BJ4" s="74"/>
+      <c r="BK4" s="75"/>
+      <c r="BL4" s="73">
         <f>BL5</f>
         <v>43794</v>
       </c>
-      <c r="BM4" s="73"/>
-      <c r="BN4" s="73"/>
-      <c r="BO4" s="73"/>
-      <c r="BP4" s="73"/>
-      <c r="BQ4" s="73"/>
-      <c r="BR4" s="74"/>
-      <c r="BS4" s="72">
+      <c r="BM4" s="74"/>
+      <c r="BN4" s="74"/>
+      <c r="BO4" s="74"/>
+      <c r="BP4" s="74"/>
+      <c r="BQ4" s="74"/>
+      <c r="BR4" s="75"/>
+      <c r="BS4" s="73">
         <f>BS5</f>
         <v>43801</v>
       </c>
-      <c r="BT4" s="73"/>
-      <c r="BU4" s="73"/>
-      <c r="BV4" s="73"/>
-      <c r="BW4" s="73"/>
-      <c r="BX4" s="73"/>
-      <c r="BY4" s="74"/>
-      <c r="BZ4" s="72">
+      <c r="BT4" s="74"/>
+      <c r="BU4" s="74"/>
+      <c r="BV4" s="74"/>
+      <c r="BW4" s="74"/>
+      <c r="BX4" s="74"/>
+      <c r="BY4" s="75"/>
+      <c r="BZ4" s="73">
         <f>BZ5</f>
         <v>43808</v>
       </c>
-      <c r="CA4" s="73"/>
-      <c r="CB4" s="73"/>
-      <c r="CC4" s="73"/>
-      <c r="CD4" s="73"/>
-      <c r="CE4" s="73"/>
-      <c r="CF4" s="74"/>
-      <c r="CG4" s="72">
+      <c r="CA4" s="74"/>
+      <c r="CB4" s="74"/>
+      <c r="CC4" s="74"/>
+      <c r="CD4" s="74"/>
+      <c r="CE4" s="74"/>
+      <c r="CF4" s="75"/>
+      <c r="CG4" s="73">
         <f>CG5</f>
         <v>43815</v>
       </c>
-      <c r="CH4" s="73"/>
-      <c r="CI4" s="73"/>
-      <c r="CJ4" s="73"/>
-      <c r="CK4" s="73"/>
-      <c r="CL4" s="73"/>
-      <c r="CM4" s="74"/>
-      <c r="CN4" s="72">
+      <c r="CH4" s="74"/>
+      <c r="CI4" s="74"/>
+      <c r="CJ4" s="74"/>
+      <c r="CK4" s="74"/>
+      <c r="CL4" s="74"/>
+      <c r="CM4" s="75"/>
+      <c r="CN4" s="73">
         <f>CN5</f>
         <v>43822</v>
       </c>
-      <c r="CO4" s="73"/>
-      <c r="CP4" s="73"/>
-      <c r="CQ4" s="73"/>
-      <c r="CR4" s="73"/>
-      <c r="CS4" s="73"/>
-      <c r="CT4" s="74"/>
-      <c r="CU4" s="72">
+      <c r="CO4" s="74"/>
+      <c r="CP4" s="74"/>
+      <c r="CQ4" s="74"/>
+      <c r="CR4" s="74"/>
+      <c r="CS4" s="74"/>
+      <c r="CT4" s="75"/>
+      <c r="CU4" s="73">
         <f>CU5</f>
         <v>43829</v>
       </c>
-      <c r="CV4" s="73"/>
-      <c r="CW4" s="73"/>
-      <c r="CX4" s="73"/>
-      <c r="CY4" s="73"/>
-      <c r="CZ4" s="73"/>
-      <c r="DA4" s="74"/>
-      <c r="DB4" s="72">
+      <c r="CV4" s="74"/>
+      <c r="CW4" s="74"/>
+      <c r="CX4" s="74"/>
+      <c r="CY4" s="74"/>
+      <c r="CZ4" s="74"/>
+      <c r="DA4" s="75"/>
+      <c r="DB4" s="73">
         <f>DB5</f>
         <v>43836</v>
       </c>
-      <c r="DC4" s="73"/>
-      <c r="DD4" s="73"/>
-      <c r="DE4" s="73"/>
-      <c r="DF4" s="73"/>
-      <c r="DG4" s="73"/>
-      <c r="DH4" s="74"/>
-      <c r="DI4" s="72">
+      <c r="DC4" s="74"/>
+      <c r="DD4" s="74"/>
+      <c r="DE4" s="74"/>
+      <c r="DF4" s="74"/>
+      <c r="DG4" s="74"/>
+      <c r="DH4" s="75"/>
+      <c r="DI4" s="73">
         <f>DI5</f>
         <v>43843</v>
       </c>
-      <c r="DJ4" s="73"/>
-      <c r="DK4" s="73"/>
-      <c r="DL4" s="73"/>
-      <c r="DM4" s="73"/>
-      <c r="DN4" s="73"/>
-      <c r="DO4" s="74"/>
-      <c r="DP4" s="72">
+      <c r="DJ4" s="74"/>
+      <c r="DK4" s="74"/>
+      <c r="DL4" s="74"/>
+      <c r="DM4" s="74"/>
+      <c r="DN4" s="74"/>
+      <c r="DO4" s="75"/>
+      <c r="DP4" s="73">
         <f>DP5</f>
         <v>43850</v>
       </c>
-      <c r="DQ4" s="73"/>
-      <c r="DR4" s="73"/>
-      <c r="DS4" s="73"/>
-      <c r="DT4" s="73"/>
-      <c r="DU4" s="73"/>
-      <c r="DV4" s="74"/>
-      <c r="DW4" s="72">
+      <c r="DQ4" s="74"/>
+      <c r="DR4" s="74"/>
+      <c r="DS4" s="74"/>
+      <c r="DT4" s="74"/>
+      <c r="DU4" s="74"/>
+      <c r="DV4" s="75"/>
+      <c r="DW4" s="73">
         <f>DW5</f>
         <v>43857</v>
       </c>
-      <c r="DX4" s="73"/>
-      <c r="DY4" s="73"/>
-      <c r="DZ4" s="73"/>
-      <c r="EA4" s="73"/>
-      <c r="EB4" s="73"/>
-      <c r="EC4" s="74"/>
-      <c r="ED4" s="72">
+      <c r="DX4" s="74"/>
+      <c r="DY4" s="74"/>
+      <c r="DZ4" s="74"/>
+      <c r="EA4" s="74"/>
+      <c r="EB4" s="74"/>
+      <c r="EC4" s="75"/>
+      <c r="ED4" s="73">
         <f>ED5</f>
         <v>43864</v>
       </c>
-      <c r="EE4" s="73"/>
-      <c r="EF4" s="73"/>
-      <c r="EG4" s="73"/>
-      <c r="EH4" s="73"/>
-      <c r="EI4" s="73"/>
-      <c r="EJ4" s="74"/>
-      <c r="EK4" s="72">
+      <c r="EE4" s="74"/>
+      <c r="EF4" s="74"/>
+      <c r="EG4" s="74"/>
+      <c r="EH4" s="74"/>
+      <c r="EI4" s="74"/>
+      <c r="EJ4" s="75"/>
+      <c r="EK4" s="73">
         <f>EK5</f>
         <v>43871</v>
       </c>
-      <c r="EL4" s="73"/>
-      <c r="EM4" s="73"/>
-      <c r="EN4" s="73"/>
-      <c r="EO4" s="73"/>
-      <c r="EP4" s="73"/>
-      <c r="EQ4" s="74"/>
-      <c r="ER4" s="72">
+      <c r="EL4" s="74"/>
+      <c r="EM4" s="74"/>
+      <c r="EN4" s="74"/>
+      <c r="EO4" s="74"/>
+      <c r="EP4" s="74"/>
+      <c r="EQ4" s="75"/>
+      <c r="ER4" s="73">
         <f>ER5</f>
         <v>43878</v>
       </c>
-      <c r="ES4" s="73"/>
-      <c r="ET4" s="73"/>
-      <c r="EU4" s="73"/>
-      <c r="EV4" s="73"/>
-      <c r="EW4" s="73"/>
-      <c r="EX4" s="74"/>
-      <c r="EY4" s="72">
+      <c r="ES4" s="74"/>
+      <c r="ET4" s="74"/>
+      <c r="EU4" s="74"/>
+      <c r="EV4" s="74"/>
+      <c r="EW4" s="74"/>
+      <c r="EX4" s="75"/>
+      <c r="EY4" s="73">
         <f>EY5</f>
         <v>43885</v>
       </c>
-      <c r="EZ4" s="73"/>
-      <c r="FA4" s="73"/>
-      <c r="FB4" s="73"/>
-      <c r="FC4" s="73"/>
-      <c r="FD4" s="73"/>
-      <c r="FE4" s="74"/>
-      <c r="FF4" s="72">
+      <c r="EZ4" s="74"/>
+      <c r="FA4" s="74"/>
+      <c r="FB4" s="74"/>
+      <c r="FC4" s="74"/>
+      <c r="FD4" s="74"/>
+      <c r="FE4" s="75"/>
+      <c r="FF4" s="73">
         <f>FF5</f>
         <v>43892</v>
       </c>
-      <c r="FG4" s="73"/>
-      <c r="FH4" s="73"/>
-      <c r="FI4" s="73"/>
-      <c r="FJ4" s="73"/>
-      <c r="FK4" s="73"/>
-      <c r="FL4" s="74"/>
-      <c r="FM4" s="72">
+      <c r="FG4" s="74"/>
+      <c r="FH4" s="74"/>
+      <c r="FI4" s="74"/>
+      <c r="FJ4" s="74"/>
+      <c r="FK4" s="74"/>
+      <c r="FL4" s="75"/>
+      <c r="FM4" s="73">
         <f>FM5</f>
         <v>43899</v>
       </c>
-      <c r="FN4" s="73"/>
-      <c r="FO4" s="73"/>
-      <c r="FP4" s="73"/>
-      <c r="FQ4" s="73"/>
-      <c r="FR4" s="73"/>
-      <c r="FS4" s="74"/>
-      <c r="FT4" s="72">
+      <c r="FN4" s="74"/>
+      <c r="FO4" s="74"/>
+      <c r="FP4" s="74"/>
+      <c r="FQ4" s="74"/>
+      <c r="FR4" s="74"/>
+      <c r="FS4" s="75"/>
+      <c r="FT4" s="73">
         <f>FT5</f>
         <v>43906</v>
       </c>
-      <c r="FU4" s="73"/>
-      <c r="FV4" s="73"/>
-      <c r="FW4" s="73"/>
-      <c r="FX4" s="73"/>
-      <c r="FY4" s="73"/>
-      <c r="FZ4" s="74"/>
-      <c r="GA4" s="72">
+      <c r="FU4" s="74"/>
+      <c r="FV4" s="74"/>
+      <c r="FW4" s="74"/>
+      <c r="FX4" s="74"/>
+      <c r="FY4" s="74"/>
+      <c r="FZ4" s="75"/>
+      <c r="GA4" s="73">
         <f>GA5</f>
         <v>43913</v>
       </c>
-      <c r="GB4" s="73"/>
-      <c r="GC4" s="73"/>
-      <c r="GD4" s="73"/>
-      <c r="GE4" s="73"/>
-      <c r="GF4" s="73"/>
-      <c r="GG4" s="74"/>
-      <c r="GH4" s="72">
+      <c r="GB4" s="74"/>
+      <c r="GC4" s="74"/>
+      <c r="GD4" s="74"/>
+      <c r="GE4" s="74"/>
+      <c r="GF4" s="74"/>
+      <c r="GG4" s="75"/>
+      <c r="GH4" s="73">
         <f>GH5</f>
         <v>43920</v>
       </c>
-      <c r="GI4" s="73"/>
-      <c r="GJ4" s="73"/>
-      <c r="GK4" s="73"/>
-      <c r="GL4" s="73"/>
-      <c r="GM4" s="73"/>
-      <c r="GN4" s="74"/>
-      <c r="GO4" s="72">
+      <c r="GI4" s="74"/>
+      <c r="GJ4" s="74"/>
+      <c r="GK4" s="74"/>
+      <c r="GL4" s="74"/>
+      <c r="GM4" s="74"/>
+      <c r="GN4" s="75"/>
+      <c r="GO4" s="73">
         <f>GO5</f>
         <v>43927</v>
       </c>
-      <c r="GP4" s="73"/>
-      <c r="GQ4" s="73"/>
-      <c r="GR4" s="73"/>
-      <c r="GS4" s="73"/>
-      <c r="GT4" s="73"/>
-      <c r="GU4" s="74"/>
+      <c r="GP4" s="74"/>
+      <c r="GQ4" s="74"/>
+      <c r="GR4" s="74"/>
+      <c r="GS4" s="74"/>
+      <c r="GT4" s="74"/>
+      <c r="GU4" s="75"/>
     </row>
     <row r="5" spans="1:203" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
       <c r="H5" s="56">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43738</v>
@@ -4010,7 +4013,7 @@
       <c r="E8" s="42"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11" t="str">
-        <f t="shared" ref="G8:G28" si="109">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="G8:G29" si="109">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="H8" s="18"/>
@@ -4649,20 +4652,19 @@
       <c r="GU10" s="18"/>
     </row>
     <row r="11" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="45"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="60">
+        <v>0.7</v>
+      </c>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43">
+        <v>43782</v>
+      </c>
       <c r="F11" s="11"/>
-      <c r="G11" s="11" t="str">
-        <f t="shared" si="109"/>
-        <v/>
-      </c>
+      <c r="G11" s="11"/>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
@@ -4675,8 +4677,8 @@
       <c r="Q11" s="18"/>
       <c r="R11" s="18"/>
       <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
       <c r="V11" s="18"/>
       <c r="W11" s="18"/>
       <c r="X11" s="18"/>
@@ -4861,23 +4863,19 @@
       <c r="GU11" s="18"/>
     </row>
     <row r="12" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="31"/>
-      <c r="B12" s="70" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="62"/>
-      <c r="D12" s="46">
-        <f>E9+1</f>
-        <v>43759</v>
-      </c>
-      <c r="E12" s="46">
-        <f>D12+14</f>
-        <v>43773</v>
-      </c>
+      <c r="A12" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="61"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="45"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="11">
+      <c r="G12" s="11" t="str">
         <f t="shared" si="109"/>
-        <v>15</v>
+        <v/>
       </c>
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
@@ -5077,18 +5075,18 @@
       <c r="GU12" s="18"/>
     </row>
     <row r="13" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30"/>
+      <c r="A13" s="31"/>
       <c r="B13" s="70" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="62"/>
       <c r="D13" s="46">
-        <f t="shared" ref="D13:D14" si="110">E12+1</f>
-        <v>43774</v>
+        <f>E9+1</f>
+        <v>43759</v>
       </c>
       <c r="E13" s="46">
         <f>D13+14</f>
-        <v>43788</v>
+        <v>43773</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11">
@@ -5107,8 +5105,8 @@
       <c r="Q13" s="18"/>
       <c r="R13" s="18"/>
       <c r="S13" s="18"/>
-      <c r="T13" s="19"/>
-      <c r="U13" s="19"/>
+      <c r="T13" s="18"/>
+      <c r="U13" s="18"/>
       <c r="V13" s="18"/>
       <c r="W13" s="18"/>
       <c r="X13" s="18"/>
@@ -5295,16 +5293,16 @@
     <row r="14" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30"/>
       <c r="B14" s="70" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C14" s="62"/>
       <c r="D14" s="46">
-        <f t="shared" si="110"/>
-        <v>43789</v>
+        <f t="shared" ref="D14:D15" si="110">E13+1</f>
+        <v>43774</v>
       </c>
       <c r="E14" s="46">
         <f>D14+14</f>
-        <v>43803</v>
+        <v>43788</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="11">
@@ -5323,8 +5321,8 @@
       <c r="Q14" s="18"/>
       <c r="R14" s="18"/>
       <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
       <c r="V14" s="18"/>
       <c r="W14" s="18"/>
       <c r="X14" s="18"/>
@@ -5509,19 +5507,23 @@
       <c r="GU14" s="18"/>
     </row>
     <row r="15" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="63"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="48"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="62"/>
+      <c r="D15" s="46">
+        <f t="shared" si="110"/>
+        <v>43789</v>
+      </c>
+      <c r="E15" s="46">
+        <f>D15+14</f>
+        <v>43803</v>
+      </c>
       <c r="F15" s="11"/>
-      <c r="G15" s="11" t="str">
+      <c r="G15" s="11">
         <f t="shared" si="109"/>
-        <v/>
+        <v>15</v>
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
@@ -5721,13 +5723,15 @@
       <c r="GU15" s="18"/>
     </row>
     <row r="16" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="30"/>
-      <c r="B16" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="64"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
+      <c r="A16" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="63"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="48"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11" t="str">
         <f t="shared" si="109"/>
@@ -5933,7 +5937,7 @@
     <row r="17" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="30"/>
       <c r="B17" s="71" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" s="64"/>
       <c r="D17" s="49"/>
@@ -6143,7 +6147,7 @@
     <row r="18" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="30"/>
       <c r="B18" s="71" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" s="64"/>
       <c r="D18" s="49"/>
@@ -6353,7 +6357,7 @@
     <row r="19" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30"/>
       <c r="B19" s="71" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19" s="64"/>
       <c r="D19" s="49"/>
@@ -6563,7 +6567,7 @@
     <row r="20" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="30"/>
       <c r="B20" s="71" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C20" s="64"/>
       <c r="D20" s="49"/>
@@ -6771,15 +6775,13 @@
       <c r="GU20" s="18"/>
     </row>
     <row r="21" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="65"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="51"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="71" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="64"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11" t="str">
         <f t="shared" si="109"/>
@@ -6983,13 +6985,15 @@
       <c r="GU21" s="18"/>
     </row>
     <row r="22" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="30"/>
-      <c r="B22" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="66"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
+      <c r="A22" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="65"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="51"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11" t="str">
         <f t="shared" si="109"/>
@@ -7195,7 +7199,7 @@
     <row r="23" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="30"/>
       <c r="B23" s="37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23" s="66"/>
       <c r="D23" s="52"/>
@@ -7405,7 +7409,7 @@
     <row r="24" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="30"/>
       <c r="B24" s="37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" s="66"/>
       <c r="D24" s="52"/>
@@ -7615,7 +7619,7 @@
     <row r="25" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="30"/>
       <c r="B25" s="37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25" s="66"/>
       <c r="D25" s="52"/>
@@ -7825,7 +7829,7 @@
     <row r="26" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="30"/>
       <c r="B26" s="37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" s="66"/>
       <c r="D26" s="52"/>
@@ -8033,13 +8037,13 @@
       <c r="GU26" s="18"/>
     </row>
     <row r="27" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="66"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="52"/>
       <c r="F27" s="11"/>
       <c r="G27" s="11" t="str">
         <f t="shared" si="109"/>
@@ -8243,257 +8247,467 @@
       <c r="GU27" s="18"/>
     </row>
     <row r="28" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="68"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17" t="str">
+      <c r="A28" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="38"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11" t="str">
         <f t="shared" si="109"/>
         <v/>
       </c>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="20"/>
-      <c r="O28" s="20"/>
-      <c r="P28" s="20"/>
-      <c r="Q28" s="20"/>
-      <c r="R28" s="20"/>
-      <c r="S28" s="20"/>
-      <c r="T28" s="20"/>
-      <c r="U28" s="20"/>
-      <c r="V28" s="20"/>
-      <c r="W28" s="20"/>
-      <c r="X28" s="20"/>
-      <c r="Y28" s="20"/>
-      <c r="Z28" s="20"/>
-      <c r="AA28" s="20"/>
-      <c r="AB28" s="20"/>
-      <c r="AC28" s="20"/>
-      <c r="AD28" s="20"/>
-      <c r="AE28" s="20"/>
-      <c r="AF28" s="20"/>
-      <c r="AG28" s="20"/>
-      <c r="AH28" s="20"/>
-      <c r="AI28" s="20"/>
-      <c r="AJ28" s="20"/>
-      <c r="AK28" s="20"/>
-      <c r="AL28" s="20"/>
-      <c r="AM28" s="20"/>
-      <c r="AN28" s="20"/>
-      <c r="AO28" s="20"/>
-      <c r="AP28" s="20"/>
-      <c r="AQ28" s="20"/>
-      <c r="AR28" s="20"/>
-      <c r="AS28" s="20"/>
-      <c r="AT28" s="20"/>
-      <c r="AU28" s="20"/>
-      <c r="AV28" s="20"/>
-      <c r="AW28" s="20"/>
-      <c r="AX28" s="20"/>
-      <c r="AY28" s="20"/>
-      <c r="AZ28" s="20"/>
-      <c r="BA28" s="20"/>
-      <c r="BB28" s="20"/>
-      <c r="BC28" s="20"/>
-      <c r="BD28" s="20"/>
-      <c r="BE28" s="20"/>
-      <c r="BF28" s="20"/>
-      <c r="BG28" s="20"/>
-      <c r="BH28" s="20"/>
-      <c r="BI28" s="20"/>
-      <c r="BJ28" s="20"/>
-      <c r="BK28" s="20"/>
-      <c r="BL28" s="20"/>
-      <c r="BM28" s="20"/>
-      <c r="BN28" s="20"/>
-      <c r="BO28" s="20"/>
-      <c r="BP28" s="20"/>
-      <c r="BQ28" s="20"/>
-      <c r="BR28" s="20"/>
-      <c r="BS28" s="20"/>
-      <c r="BT28" s="20"/>
-      <c r="BU28" s="20"/>
-      <c r="BV28" s="20"/>
-      <c r="BW28" s="20"/>
-      <c r="BX28" s="20"/>
-      <c r="BY28" s="20"/>
-      <c r="BZ28" s="20"/>
-      <c r="CA28" s="20"/>
-      <c r="CB28" s="20"/>
-      <c r="CC28" s="20"/>
-      <c r="CD28" s="20"/>
-      <c r="CE28" s="20"/>
-      <c r="CF28" s="20"/>
-      <c r="CG28" s="20"/>
-      <c r="CH28" s="20"/>
-      <c r="CI28" s="20"/>
-      <c r="CJ28" s="20"/>
-      <c r="CK28" s="20"/>
-      <c r="CL28" s="20"/>
-      <c r="CM28" s="20"/>
-      <c r="CN28" s="20"/>
-      <c r="CO28" s="20"/>
-      <c r="CP28" s="20"/>
-      <c r="CQ28" s="20"/>
-      <c r="CR28" s="20"/>
-      <c r="CS28" s="20"/>
-      <c r="CT28" s="20"/>
-      <c r="CU28" s="20"/>
-      <c r="CV28" s="20"/>
-      <c r="CW28" s="20"/>
-      <c r="CX28" s="20"/>
-      <c r="CY28" s="20"/>
-      <c r="CZ28" s="20"/>
-      <c r="DA28" s="20"/>
-      <c r="DB28" s="20"/>
-      <c r="DC28" s="20"/>
-      <c r="DD28" s="20"/>
-      <c r="DE28" s="20"/>
-      <c r="DF28" s="20"/>
-      <c r="DG28" s="20"/>
-      <c r="DH28" s="20"/>
-      <c r="DI28" s="20"/>
-      <c r="DJ28" s="20"/>
-      <c r="DK28" s="20"/>
-      <c r="DL28" s="20"/>
-      <c r="DM28" s="20"/>
-      <c r="DN28" s="20"/>
-      <c r="DO28" s="20"/>
-      <c r="DP28" s="20"/>
-      <c r="DQ28" s="20"/>
-      <c r="DR28" s="20"/>
-      <c r="DS28" s="20"/>
-      <c r="DT28" s="20"/>
-      <c r="DU28" s="20"/>
-      <c r="DV28" s="20"/>
-      <c r="DW28" s="20"/>
-      <c r="DX28" s="20"/>
-      <c r="DY28" s="20"/>
-      <c r="DZ28" s="20"/>
-      <c r="EA28" s="20"/>
-      <c r="EB28" s="20"/>
-      <c r="EC28" s="20"/>
-      <c r="ED28" s="20"/>
-      <c r="EE28" s="20"/>
-      <c r="EF28" s="20"/>
-      <c r="EG28" s="20"/>
-      <c r="EH28" s="20"/>
-      <c r="EI28" s="20"/>
-      <c r="EJ28" s="20"/>
-      <c r="EK28" s="20"/>
-      <c r="EL28" s="20"/>
-      <c r="EM28" s="20"/>
-      <c r="EN28" s="20"/>
-      <c r="EO28" s="20"/>
-      <c r="EP28" s="20"/>
-      <c r="EQ28" s="20"/>
-      <c r="ER28" s="20"/>
-      <c r="ES28" s="20"/>
-      <c r="ET28" s="20"/>
-      <c r="EU28" s="20"/>
-      <c r="EV28" s="20"/>
-      <c r="EW28" s="20"/>
-      <c r="EX28" s="20"/>
-      <c r="EY28" s="20"/>
-      <c r="EZ28" s="20"/>
-      <c r="FA28" s="20"/>
-      <c r="FB28" s="20"/>
-      <c r="FC28" s="20"/>
-      <c r="FD28" s="20"/>
-      <c r="FE28" s="20"/>
-      <c r="FF28" s="20"/>
-      <c r="FG28" s="20"/>
-      <c r="FH28" s="20"/>
-      <c r="FI28" s="20"/>
-      <c r="FJ28" s="20"/>
-      <c r="FK28" s="20"/>
-      <c r="FL28" s="20"/>
-      <c r="FM28" s="20"/>
-      <c r="FN28" s="20"/>
-      <c r="FO28" s="20"/>
-      <c r="FP28" s="20"/>
-      <c r="FQ28" s="20"/>
-      <c r="FR28" s="20"/>
-      <c r="FS28" s="20"/>
-      <c r="FT28" s="20"/>
-      <c r="FU28" s="20"/>
-      <c r="FV28" s="20"/>
-      <c r="FW28" s="20"/>
-      <c r="FX28" s="20"/>
-      <c r="FY28" s="20"/>
-      <c r="FZ28" s="20"/>
-      <c r="GA28" s="20"/>
-      <c r="GB28" s="20"/>
-      <c r="GC28" s="20"/>
-      <c r="GD28" s="20"/>
-      <c r="GE28" s="20"/>
-      <c r="GF28" s="20"/>
-      <c r="GG28" s="20"/>
-      <c r="GH28" s="20"/>
-      <c r="GI28" s="20"/>
-      <c r="GJ28" s="20"/>
-      <c r="GK28" s="20"/>
-      <c r="GL28" s="20"/>
-      <c r="GM28" s="20"/>
-      <c r="GN28" s="20"/>
-      <c r="GO28" s="20"/>
-      <c r="GP28" s="20"/>
-      <c r="GQ28" s="20"/>
-      <c r="GR28" s="20"/>
-      <c r="GS28" s="20"/>
-      <c r="GT28" s="20"/>
-      <c r="GU28" s="20"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="18"/>
+      <c r="T28" s="18"/>
+      <c r="U28" s="18"/>
+      <c r="V28" s="18"/>
+      <c r="W28" s="18"/>
+      <c r="X28" s="18"/>
+      <c r="Y28" s="18"/>
+      <c r="Z28" s="18"/>
+      <c r="AA28" s="18"/>
+      <c r="AB28" s="18"/>
+      <c r="AC28" s="18"/>
+      <c r="AD28" s="18"/>
+      <c r="AE28" s="18"/>
+      <c r="AF28" s="18"/>
+      <c r="AG28" s="18"/>
+      <c r="AH28" s="18"/>
+      <c r="AI28" s="18"/>
+      <c r="AJ28" s="18"/>
+      <c r="AK28" s="18"/>
+      <c r="AL28" s="18"/>
+      <c r="AM28" s="18"/>
+      <c r="AN28" s="18"/>
+      <c r="AO28" s="18"/>
+      <c r="AP28" s="18"/>
+      <c r="AQ28" s="18"/>
+      <c r="AR28" s="18"/>
+      <c r="AS28" s="18"/>
+      <c r="AT28" s="18"/>
+      <c r="AU28" s="18"/>
+      <c r="AV28" s="18"/>
+      <c r="AW28" s="18"/>
+      <c r="AX28" s="18"/>
+      <c r="AY28" s="18"/>
+      <c r="AZ28" s="18"/>
+      <c r="BA28" s="18"/>
+      <c r="BB28" s="18"/>
+      <c r="BC28" s="18"/>
+      <c r="BD28" s="18"/>
+      <c r="BE28" s="18"/>
+      <c r="BF28" s="18"/>
+      <c r="BG28" s="18"/>
+      <c r="BH28" s="18"/>
+      <c r="BI28" s="18"/>
+      <c r="BJ28" s="18"/>
+      <c r="BK28" s="18"/>
+      <c r="BL28" s="18"/>
+      <c r="BM28" s="18"/>
+      <c r="BN28" s="18"/>
+      <c r="BO28" s="18"/>
+      <c r="BP28" s="18"/>
+      <c r="BQ28" s="18"/>
+      <c r="BR28" s="18"/>
+      <c r="BS28" s="18"/>
+      <c r="BT28" s="18"/>
+      <c r="BU28" s="18"/>
+      <c r="BV28" s="18"/>
+      <c r="BW28" s="18"/>
+      <c r="BX28" s="18"/>
+      <c r="BY28" s="18"/>
+      <c r="BZ28" s="18"/>
+      <c r="CA28" s="18"/>
+      <c r="CB28" s="18"/>
+      <c r="CC28" s="18"/>
+      <c r="CD28" s="18"/>
+      <c r="CE28" s="18"/>
+      <c r="CF28" s="18"/>
+      <c r="CG28" s="18"/>
+      <c r="CH28" s="18"/>
+      <c r="CI28" s="18"/>
+      <c r="CJ28" s="18"/>
+      <c r="CK28" s="18"/>
+      <c r="CL28" s="18"/>
+      <c r="CM28" s="18"/>
+      <c r="CN28" s="18"/>
+      <c r="CO28" s="18"/>
+      <c r="CP28" s="18"/>
+      <c r="CQ28" s="18"/>
+      <c r="CR28" s="18"/>
+      <c r="CS28" s="18"/>
+      <c r="CT28" s="18"/>
+      <c r="CU28" s="18"/>
+      <c r="CV28" s="18"/>
+      <c r="CW28" s="18"/>
+      <c r="CX28" s="18"/>
+      <c r="CY28" s="18"/>
+      <c r="CZ28" s="18"/>
+      <c r="DA28" s="18"/>
+      <c r="DB28" s="18"/>
+      <c r="DC28" s="18"/>
+      <c r="DD28" s="18"/>
+      <c r="DE28" s="18"/>
+      <c r="DF28" s="18"/>
+      <c r="DG28" s="18"/>
+      <c r="DH28" s="18"/>
+      <c r="DI28" s="18"/>
+      <c r="DJ28" s="18"/>
+      <c r="DK28" s="18"/>
+      <c r="DL28" s="18"/>
+      <c r="DM28" s="18"/>
+      <c r="DN28" s="18"/>
+      <c r="DO28" s="18"/>
+      <c r="DP28" s="18"/>
+      <c r="DQ28" s="18"/>
+      <c r="DR28" s="18"/>
+      <c r="DS28" s="18"/>
+      <c r="DT28" s="18"/>
+      <c r="DU28" s="18"/>
+      <c r="DV28" s="18"/>
+      <c r="DW28" s="18"/>
+      <c r="DX28" s="18"/>
+      <c r="DY28" s="18"/>
+      <c r="DZ28" s="18"/>
+      <c r="EA28" s="18"/>
+      <c r="EB28" s="18"/>
+      <c r="EC28" s="18"/>
+      <c r="ED28" s="18"/>
+      <c r="EE28" s="18"/>
+      <c r="EF28" s="18"/>
+      <c r="EG28" s="18"/>
+      <c r="EH28" s="18"/>
+      <c r="EI28" s="18"/>
+      <c r="EJ28" s="18"/>
+      <c r="EK28" s="18"/>
+      <c r="EL28" s="18"/>
+      <c r="EM28" s="18"/>
+      <c r="EN28" s="18"/>
+      <c r="EO28" s="18"/>
+      <c r="EP28" s="18"/>
+      <c r="EQ28" s="18"/>
+      <c r="ER28" s="18"/>
+      <c r="ES28" s="18"/>
+      <c r="ET28" s="18"/>
+      <c r="EU28" s="18"/>
+      <c r="EV28" s="18"/>
+      <c r="EW28" s="18"/>
+      <c r="EX28" s="18"/>
+      <c r="EY28" s="18"/>
+      <c r="EZ28" s="18"/>
+      <c r="FA28" s="18"/>
+      <c r="FB28" s="18"/>
+      <c r="FC28" s="18"/>
+      <c r="FD28" s="18"/>
+      <c r="FE28" s="18"/>
+      <c r="FF28" s="18"/>
+      <c r="FG28" s="18"/>
+      <c r="FH28" s="18"/>
+      <c r="FI28" s="18"/>
+      <c r="FJ28" s="18"/>
+      <c r="FK28" s="18"/>
+      <c r="FL28" s="18"/>
+      <c r="FM28" s="18"/>
+      <c r="FN28" s="18"/>
+      <c r="FO28" s="18"/>
+      <c r="FP28" s="18"/>
+      <c r="FQ28" s="18"/>
+      <c r="FR28" s="18"/>
+      <c r="FS28" s="18"/>
+      <c r="FT28" s="18"/>
+      <c r="FU28" s="18"/>
+      <c r="FV28" s="18"/>
+      <c r="FW28" s="18"/>
+      <c r="FX28" s="18"/>
+      <c r="FY28" s="18"/>
+      <c r="FZ28" s="18"/>
+      <c r="GA28" s="18"/>
+      <c r="GB28" s="18"/>
+      <c r="GC28" s="18"/>
+      <c r="GD28" s="18"/>
+      <c r="GE28" s="18"/>
+      <c r="GF28" s="18"/>
+      <c r="GG28" s="18"/>
+      <c r="GH28" s="18"/>
+      <c r="GI28" s="18"/>
+      <c r="GJ28" s="18"/>
+      <c r="GK28" s="18"/>
+      <c r="GL28" s="18"/>
+      <c r="GM28" s="18"/>
+      <c r="GN28" s="18"/>
+      <c r="GO28" s="18"/>
+      <c r="GP28" s="18"/>
+      <c r="GQ28" s="18"/>
+      <c r="GR28" s="18"/>
+      <c r="GS28" s="18"/>
+      <c r="GT28" s="18"/>
+      <c r="GU28" s="18"/>
     </row>
-    <row r="29" spans="1:203" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F29" s="5"/>
+    <row r="29" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="68"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17" t="str">
+        <f t="shared" si="109"/>
+        <v/>
+      </c>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
+      <c r="Q29" s="20"/>
+      <c r="R29" s="20"/>
+      <c r="S29" s="20"/>
+      <c r="T29" s="20"/>
+      <c r="U29" s="20"/>
+      <c r="V29" s="20"/>
+      <c r="W29" s="20"/>
+      <c r="X29" s="20"/>
+      <c r="Y29" s="20"/>
+      <c r="Z29" s="20"/>
+      <c r="AA29" s="20"/>
+      <c r="AB29" s="20"/>
+      <c r="AC29" s="20"/>
+      <c r="AD29" s="20"/>
+      <c r="AE29" s="20"/>
+      <c r="AF29" s="20"/>
+      <c r="AG29" s="20"/>
+      <c r="AH29" s="20"/>
+      <c r="AI29" s="20"/>
+      <c r="AJ29" s="20"/>
+      <c r="AK29" s="20"/>
+      <c r="AL29" s="20"/>
+      <c r="AM29" s="20"/>
+      <c r="AN29" s="20"/>
+      <c r="AO29" s="20"/>
+      <c r="AP29" s="20"/>
+      <c r="AQ29" s="20"/>
+      <c r="AR29" s="20"/>
+      <c r="AS29" s="20"/>
+      <c r="AT29" s="20"/>
+      <c r="AU29" s="20"/>
+      <c r="AV29" s="20"/>
+      <c r="AW29" s="20"/>
+      <c r="AX29" s="20"/>
+      <c r="AY29" s="20"/>
+      <c r="AZ29" s="20"/>
+      <c r="BA29" s="20"/>
+      <c r="BB29" s="20"/>
+      <c r="BC29" s="20"/>
+      <c r="BD29" s="20"/>
+      <c r="BE29" s="20"/>
+      <c r="BF29" s="20"/>
+      <c r="BG29" s="20"/>
+      <c r="BH29" s="20"/>
+      <c r="BI29" s="20"/>
+      <c r="BJ29" s="20"/>
+      <c r="BK29" s="20"/>
+      <c r="BL29" s="20"/>
+      <c r="BM29" s="20"/>
+      <c r="BN29" s="20"/>
+      <c r="BO29" s="20"/>
+      <c r="BP29" s="20"/>
+      <c r="BQ29" s="20"/>
+      <c r="BR29" s="20"/>
+      <c r="BS29" s="20"/>
+      <c r="BT29" s="20"/>
+      <c r="BU29" s="20"/>
+      <c r="BV29" s="20"/>
+      <c r="BW29" s="20"/>
+      <c r="BX29" s="20"/>
+      <c r="BY29" s="20"/>
+      <c r="BZ29" s="20"/>
+      <c r="CA29" s="20"/>
+      <c r="CB29" s="20"/>
+      <c r="CC29" s="20"/>
+      <c r="CD29" s="20"/>
+      <c r="CE29" s="20"/>
+      <c r="CF29" s="20"/>
+      <c r="CG29" s="20"/>
+      <c r="CH29" s="20"/>
+      <c r="CI29" s="20"/>
+      <c r="CJ29" s="20"/>
+      <c r="CK29" s="20"/>
+      <c r="CL29" s="20"/>
+      <c r="CM29" s="20"/>
+      <c r="CN29" s="20"/>
+      <c r="CO29" s="20"/>
+      <c r="CP29" s="20"/>
+      <c r="CQ29" s="20"/>
+      <c r="CR29" s="20"/>
+      <c r="CS29" s="20"/>
+      <c r="CT29" s="20"/>
+      <c r="CU29" s="20"/>
+      <c r="CV29" s="20"/>
+      <c r="CW29" s="20"/>
+      <c r="CX29" s="20"/>
+      <c r="CY29" s="20"/>
+      <c r="CZ29" s="20"/>
+      <c r="DA29" s="20"/>
+      <c r="DB29" s="20"/>
+      <c r="DC29" s="20"/>
+      <c r="DD29" s="20"/>
+      <c r="DE29" s="20"/>
+      <c r="DF29" s="20"/>
+      <c r="DG29" s="20"/>
+      <c r="DH29" s="20"/>
+      <c r="DI29" s="20"/>
+      <c r="DJ29" s="20"/>
+      <c r="DK29" s="20"/>
+      <c r="DL29" s="20"/>
+      <c r="DM29" s="20"/>
+      <c r="DN29" s="20"/>
+      <c r="DO29" s="20"/>
+      <c r="DP29" s="20"/>
+      <c r="DQ29" s="20"/>
+      <c r="DR29" s="20"/>
+      <c r="DS29" s="20"/>
+      <c r="DT29" s="20"/>
+      <c r="DU29" s="20"/>
+      <c r="DV29" s="20"/>
+      <c r="DW29" s="20"/>
+      <c r="DX29" s="20"/>
+      <c r="DY29" s="20"/>
+      <c r="DZ29" s="20"/>
+      <c r="EA29" s="20"/>
+      <c r="EB29" s="20"/>
+      <c r="EC29" s="20"/>
+      <c r="ED29" s="20"/>
+      <c r="EE29" s="20"/>
+      <c r="EF29" s="20"/>
+      <c r="EG29" s="20"/>
+      <c r="EH29" s="20"/>
+      <c r="EI29" s="20"/>
+      <c r="EJ29" s="20"/>
+      <c r="EK29" s="20"/>
+      <c r="EL29" s="20"/>
+      <c r="EM29" s="20"/>
+      <c r="EN29" s="20"/>
+      <c r="EO29" s="20"/>
+      <c r="EP29" s="20"/>
+      <c r="EQ29" s="20"/>
+      <c r="ER29" s="20"/>
+      <c r="ES29" s="20"/>
+      <c r="ET29" s="20"/>
+      <c r="EU29" s="20"/>
+      <c r="EV29" s="20"/>
+      <c r="EW29" s="20"/>
+      <c r="EX29" s="20"/>
+      <c r="EY29" s="20"/>
+      <c r="EZ29" s="20"/>
+      <c r="FA29" s="20"/>
+      <c r="FB29" s="20"/>
+      <c r="FC29" s="20"/>
+      <c r="FD29" s="20"/>
+      <c r="FE29" s="20"/>
+      <c r="FF29" s="20"/>
+      <c r="FG29" s="20"/>
+      <c r="FH29" s="20"/>
+      <c r="FI29" s="20"/>
+      <c r="FJ29" s="20"/>
+      <c r="FK29" s="20"/>
+      <c r="FL29" s="20"/>
+      <c r="FM29" s="20"/>
+      <c r="FN29" s="20"/>
+      <c r="FO29" s="20"/>
+      <c r="FP29" s="20"/>
+      <c r="FQ29" s="20"/>
+      <c r="FR29" s="20"/>
+      <c r="FS29" s="20"/>
+      <c r="FT29" s="20"/>
+      <c r="FU29" s="20"/>
+      <c r="FV29" s="20"/>
+      <c r="FW29" s="20"/>
+      <c r="FX29" s="20"/>
+      <c r="FY29" s="20"/>
+      <c r="FZ29" s="20"/>
+      <c r="GA29" s="20"/>
+      <c r="GB29" s="20"/>
+      <c r="GC29" s="20"/>
+      <c r="GD29" s="20"/>
+      <c r="GE29" s="20"/>
+      <c r="GF29" s="20"/>
+      <c r="GG29" s="20"/>
+      <c r="GH29" s="20"/>
+      <c r="GI29" s="20"/>
+      <c r="GJ29" s="20"/>
+      <c r="GK29" s="20"/>
+      <c r="GL29" s="20"/>
+      <c r="GM29" s="20"/>
+      <c r="GN29" s="20"/>
+      <c r="GO29" s="20"/>
+      <c r="GP29" s="20"/>
+      <c r="GQ29" s="20"/>
+      <c r="GR29" s="20"/>
+      <c r="GS29" s="20"/>
+      <c r="GT29" s="20"/>
+      <c r="GU29" s="20"/>
     </row>
     <row r="30" spans="1:203" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E30" s="32"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:203" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E31" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="FM4:FS4"/>
+    <mergeCell ref="FT4:FZ4"/>
+    <mergeCell ref="GA4:GG4"/>
+    <mergeCell ref="GH4:GN4"/>
+    <mergeCell ref="GO4:GU4"/>
+    <mergeCell ref="ED4:EJ4"/>
+    <mergeCell ref="EK4:EQ4"/>
+    <mergeCell ref="ER4:EX4"/>
+    <mergeCell ref="EY4:FE4"/>
+    <mergeCell ref="FF4:FL4"/>
+    <mergeCell ref="CU4:DA4"/>
+    <mergeCell ref="DB4:DH4"/>
+    <mergeCell ref="DI4:DO4"/>
+    <mergeCell ref="DP4:DV4"/>
+    <mergeCell ref="DW4:EC4"/>
+    <mergeCell ref="BL4:BR4"/>
+    <mergeCell ref="BS4:BY4"/>
+    <mergeCell ref="BZ4:CF4"/>
+    <mergeCell ref="CG4:CM4"/>
+    <mergeCell ref="CN4:CT4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="AJ4:AP4"/>
+    <mergeCell ref="AQ4:AW4"/>
+    <mergeCell ref="AX4:BD4"/>
+    <mergeCell ref="BE4:BK4"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="H4:N4"/>
     <mergeCell ref="O4:U4"/>
     <mergeCell ref="V4:AB4"/>
     <mergeCell ref="AC4:AI4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="AJ4:AP4"/>
-    <mergeCell ref="AQ4:AW4"/>
-    <mergeCell ref="AX4:BD4"/>
-    <mergeCell ref="BE4:BK4"/>
-    <mergeCell ref="BL4:BR4"/>
-    <mergeCell ref="BS4:BY4"/>
-    <mergeCell ref="BZ4:CF4"/>
-    <mergeCell ref="CG4:CM4"/>
-    <mergeCell ref="CN4:CT4"/>
-    <mergeCell ref="CU4:DA4"/>
-    <mergeCell ref="DB4:DH4"/>
-    <mergeCell ref="DI4:DO4"/>
-    <mergeCell ref="DP4:DV4"/>
-    <mergeCell ref="DW4:EC4"/>
-    <mergeCell ref="ED4:EJ4"/>
-    <mergeCell ref="EK4:EQ4"/>
-    <mergeCell ref="ER4:EX4"/>
-    <mergeCell ref="EY4:FE4"/>
-    <mergeCell ref="FF4:FL4"/>
-    <mergeCell ref="FM4:FS4"/>
-    <mergeCell ref="FT4:FZ4"/>
-    <mergeCell ref="GA4:GG4"/>
-    <mergeCell ref="GH4:GN4"/>
-    <mergeCell ref="GO4:GU4"/>
   </mergeCells>
-  <conditionalFormatting sqref="C7:C28">
+  <conditionalFormatting sqref="C7:C29">
     <cfRule type="dataBar" priority="44">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8507,12 +8721,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:GU28">
+  <conditionalFormatting sqref="H5:GU29">
     <cfRule type="expression" dxfId="2" priority="63">
       <formula>AND(TODAY()&gt;=H$5,TODAY()&lt;I$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:GU28">
+  <conditionalFormatting sqref="H7:GU29">
     <cfRule type="expression" dxfId="1" priority="57">
       <formula>AND(task_start&lt;=H$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=H$5)</formula>
     </cfRule>
@@ -8547,7 +8761,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>C7:C28</xm:sqref>
+          <xm:sqref>C7:C29</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Finished interim and got AST generation working
</commit_message>
<xml_diff>
--- a/docs/Proposal and Planning/GANTT.xlsx
+++ b/docs/Proposal and Planning/GANTT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427929E4-EE3C-47C0-9778-8E50F1630ECD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104BB033-E135-438B-BE3F-04AC9839BBEB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>Create a project schedule in this worksheet.
 Enter the title of this project in cell B1. 
@@ -233,12 +233,6 @@
     <t>Disabling ASLR on Virtual Instance</t>
   </si>
   <si>
-    <t>Testing Exploit</t>
-  </si>
-  <si>
-    <t>Writing Exploit</t>
-  </si>
-  <si>
     <t>Finishing Research</t>
   </si>
   <si>
@@ -246,6 +240,18 @@
   </si>
   <si>
     <t>Writing Interim</t>
+  </si>
+  <si>
+    <t>Writing the Exploit</t>
+  </si>
+  <si>
+    <t>Testing the Exploit</t>
+  </si>
+  <si>
+    <t>Testing the Type Checker</t>
+  </si>
+  <si>
+    <t>Testing the Code Generator</t>
   </si>
 </sst>
 </file>
@@ -1235,9 +1241,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="12" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="169" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1248,6 +1251,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="171" fontId="7" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="20% - Accent1" xfId="31" builtinId="30" customBuiltin="1"/>
@@ -1855,11 +1861,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:GU31"/>
+  <dimension ref="A1:GU33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA16" sqref="AA16"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1902,10 +1908,10 @@
       </c>
       <c r="B3" s="36"/>
       <c r="C3" s="55"/>
-      <c r="D3" s="72">
+      <c r="D3" s="76">
         <v>43738</v>
       </c>
-      <c r="E3" s="72"/>
+      <c r="E3" s="76"/>
     </row>
     <row r="4" spans="1:203" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
@@ -1915,296 +1921,296 @@
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="H4" s="73">
+      <c r="H4" s="72">
         <f>H5</f>
         <v>43738</v>
       </c>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74"/>
-      <c r="L4" s="74"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="75"/>
-      <c r="O4" s="73">
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="74"/>
+      <c r="O4" s="72">
         <f>O5</f>
         <v>43745</v>
       </c>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="74"/>
-      <c r="S4" s="74"/>
-      <c r="T4" s="74"/>
-      <c r="U4" s="75"/>
-      <c r="V4" s="73">
+      <c r="P4" s="73"/>
+      <c r="Q4" s="73"/>
+      <c r="R4" s="73"/>
+      <c r="S4" s="73"/>
+      <c r="T4" s="73"/>
+      <c r="U4" s="74"/>
+      <c r="V4" s="72">
         <f>V5</f>
         <v>43752</v>
       </c>
-      <c r="W4" s="74"/>
-      <c r="X4" s="74"/>
-      <c r="Y4" s="74"/>
-      <c r="Z4" s="74"/>
-      <c r="AA4" s="74"/>
-      <c r="AB4" s="75"/>
-      <c r="AC4" s="73">
+      <c r="W4" s="73"/>
+      <c r="X4" s="73"/>
+      <c r="Y4" s="73"/>
+      <c r="Z4" s="73"/>
+      <c r="AA4" s="73"/>
+      <c r="AB4" s="74"/>
+      <c r="AC4" s="72">
         <f>AC5</f>
         <v>43759</v>
       </c>
-      <c r="AD4" s="74"/>
-      <c r="AE4" s="74"/>
-      <c r="AF4" s="74"/>
-      <c r="AG4" s="74"/>
-      <c r="AH4" s="74"/>
-      <c r="AI4" s="75"/>
-      <c r="AJ4" s="73">
+      <c r="AD4" s="73"/>
+      <c r="AE4" s="73"/>
+      <c r="AF4" s="73"/>
+      <c r="AG4" s="73"/>
+      <c r="AH4" s="73"/>
+      <c r="AI4" s="74"/>
+      <c r="AJ4" s="72">
         <f>AJ5</f>
         <v>43766</v>
       </c>
-      <c r="AK4" s="74"/>
-      <c r="AL4" s="74"/>
-      <c r="AM4" s="74"/>
-      <c r="AN4" s="74"/>
-      <c r="AO4" s="74"/>
-      <c r="AP4" s="75"/>
-      <c r="AQ4" s="73">
+      <c r="AK4" s="73"/>
+      <c r="AL4" s="73"/>
+      <c r="AM4" s="73"/>
+      <c r="AN4" s="73"/>
+      <c r="AO4" s="73"/>
+      <c r="AP4" s="74"/>
+      <c r="AQ4" s="72">
         <f>AQ5</f>
         <v>43773</v>
       </c>
-      <c r="AR4" s="74"/>
-      <c r="AS4" s="74"/>
-      <c r="AT4" s="74"/>
-      <c r="AU4" s="74"/>
-      <c r="AV4" s="74"/>
-      <c r="AW4" s="75"/>
-      <c r="AX4" s="73">
+      <c r="AR4" s="73"/>
+      <c r="AS4" s="73"/>
+      <c r="AT4" s="73"/>
+      <c r="AU4" s="73"/>
+      <c r="AV4" s="73"/>
+      <c r="AW4" s="74"/>
+      <c r="AX4" s="72">
         <f>AX5</f>
         <v>43780</v>
       </c>
-      <c r="AY4" s="74"/>
-      <c r="AZ4" s="74"/>
-      <c r="BA4" s="74"/>
-      <c r="BB4" s="74"/>
-      <c r="BC4" s="74"/>
-      <c r="BD4" s="75"/>
-      <c r="BE4" s="73">
+      <c r="AY4" s="73"/>
+      <c r="AZ4" s="73"/>
+      <c r="BA4" s="73"/>
+      <c r="BB4" s="73"/>
+      <c r="BC4" s="73"/>
+      <c r="BD4" s="74"/>
+      <c r="BE4" s="72">
         <f>BE5</f>
         <v>43787</v>
       </c>
-      <c r="BF4" s="74"/>
-      <c r="BG4" s="74"/>
-      <c r="BH4" s="74"/>
-      <c r="BI4" s="74"/>
-      <c r="BJ4" s="74"/>
-      <c r="BK4" s="75"/>
-      <c r="BL4" s="73">
+      <c r="BF4" s="73"/>
+      <c r="BG4" s="73"/>
+      <c r="BH4" s="73"/>
+      <c r="BI4" s="73"/>
+      <c r="BJ4" s="73"/>
+      <c r="BK4" s="74"/>
+      <c r="BL4" s="72">
         <f>BL5</f>
         <v>43794</v>
       </c>
-      <c r="BM4" s="74"/>
-      <c r="BN4" s="74"/>
-      <c r="BO4" s="74"/>
-      <c r="BP4" s="74"/>
-      <c r="BQ4" s="74"/>
-      <c r="BR4" s="75"/>
-      <c r="BS4" s="73">
+      <c r="BM4" s="73"/>
+      <c r="BN4" s="73"/>
+      <c r="BO4" s="73"/>
+      <c r="BP4" s="73"/>
+      <c r="BQ4" s="73"/>
+      <c r="BR4" s="74"/>
+      <c r="BS4" s="72">
         <f>BS5</f>
         <v>43801</v>
       </c>
-      <c r="BT4" s="74"/>
-      <c r="BU4" s="74"/>
-      <c r="BV4" s="74"/>
-      <c r="BW4" s="74"/>
-      <c r="BX4" s="74"/>
-      <c r="BY4" s="75"/>
-      <c r="BZ4" s="73">
+      <c r="BT4" s="73"/>
+      <c r="BU4" s="73"/>
+      <c r="BV4" s="73"/>
+      <c r="BW4" s="73"/>
+      <c r="BX4" s="73"/>
+      <c r="BY4" s="74"/>
+      <c r="BZ4" s="72">
         <f>BZ5</f>
         <v>43808</v>
       </c>
-      <c r="CA4" s="74"/>
-      <c r="CB4" s="74"/>
-      <c r="CC4" s="74"/>
-      <c r="CD4" s="74"/>
-      <c r="CE4" s="74"/>
-      <c r="CF4" s="75"/>
-      <c r="CG4" s="73">
+      <c r="CA4" s="73"/>
+      <c r="CB4" s="73"/>
+      <c r="CC4" s="73"/>
+      <c r="CD4" s="73"/>
+      <c r="CE4" s="73"/>
+      <c r="CF4" s="74"/>
+      <c r="CG4" s="72">
         <f>CG5</f>
         <v>43815</v>
       </c>
-      <c r="CH4" s="74"/>
-      <c r="CI4" s="74"/>
-      <c r="CJ4" s="74"/>
-      <c r="CK4" s="74"/>
-      <c r="CL4" s="74"/>
-      <c r="CM4" s="75"/>
-      <c r="CN4" s="73">
+      <c r="CH4" s="73"/>
+      <c r="CI4" s="73"/>
+      <c r="CJ4" s="73"/>
+      <c r="CK4" s="73"/>
+      <c r="CL4" s="73"/>
+      <c r="CM4" s="74"/>
+      <c r="CN4" s="72">
         <f>CN5</f>
         <v>43822</v>
       </c>
-      <c r="CO4" s="74"/>
-      <c r="CP4" s="74"/>
-      <c r="CQ4" s="74"/>
-      <c r="CR4" s="74"/>
-      <c r="CS4" s="74"/>
-      <c r="CT4" s="75"/>
-      <c r="CU4" s="73">
+      <c r="CO4" s="73"/>
+      <c r="CP4" s="73"/>
+      <c r="CQ4" s="73"/>
+      <c r="CR4" s="73"/>
+      <c r="CS4" s="73"/>
+      <c r="CT4" s="74"/>
+      <c r="CU4" s="72">
         <f>CU5</f>
         <v>43829</v>
       </c>
-      <c r="CV4" s="74"/>
-      <c r="CW4" s="74"/>
-      <c r="CX4" s="74"/>
-      <c r="CY4" s="74"/>
-      <c r="CZ4" s="74"/>
-      <c r="DA4" s="75"/>
-      <c r="DB4" s="73">
+      <c r="CV4" s="73"/>
+      <c r="CW4" s="73"/>
+      <c r="CX4" s="73"/>
+      <c r="CY4" s="73"/>
+      <c r="CZ4" s="73"/>
+      <c r="DA4" s="74"/>
+      <c r="DB4" s="72">
         <f>DB5</f>
         <v>43836</v>
       </c>
-      <c r="DC4" s="74"/>
-      <c r="DD4" s="74"/>
-      <c r="DE4" s="74"/>
-      <c r="DF4" s="74"/>
-      <c r="DG4" s="74"/>
-      <c r="DH4" s="75"/>
-      <c r="DI4" s="73">
+      <c r="DC4" s="73"/>
+      <c r="DD4" s="73"/>
+      <c r="DE4" s="73"/>
+      <c r="DF4" s="73"/>
+      <c r="DG4" s="73"/>
+      <c r="DH4" s="74"/>
+      <c r="DI4" s="72">
         <f>DI5</f>
         <v>43843</v>
       </c>
-      <c r="DJ4" s="74"/>
-      <c r="DK4" s="74"/>
-      <c r="DL4" s="74"/>
-      <c r="DM4" s="74"/>
-      <c r="DN4" s="74"/>
-      <c r="DO4" s="75"/>
-      <c r="DP4" s="73">
+      <c r="DJ4" s="73"/>
+      <c r="DK4" s="73"/>
+      <c r="DL4" s="73"/>
+      <c r="DM4" s="73"/>
+      <c r="DN4" s="73"/>
+      <c r="DO4" s="74"/>
+      <c r="DP4" s="72">
         <f>DP5</f>
         <v>43850</v>
       </c>
-      <c r="DQ4" s="74"/>
-      <c r="DR4" s="74"/>
-      <c r="DS4" s="74"/>
-      <c r="DT4" s="74"/>
-      <c r="DU4" s="74"/>
-      <c r="DV4" s="75"/>
-      <c r="DW4" s="73">
+      <c r="DQ4" s="73"/>
+      <c r="DR4" s="73"/>
+      <c r="DS4" s="73"/>
+      <c r="DT4" s="73"/>
+      <c r="DU4" s="73"/>
+      <c r="DV4" s="74"/>
+      <c r="DW4" s="72">
         <f>DW5</f>
         <v>43857</v>
       </c>
-      <c r="DX4" s="74"/>
-      <c r="DY4" s="74"/>
-      <c r="DZ4" s="74"/>
-      <c r="EA4" s="74"/>
-      <c r="EB4" s="74"/>
-      <c r="EC4" s="75"/>
-      <c r="ED4" s="73">
+      <c r="DX4" s="73"/>
+      <c r="DY4" s="73"/>
+      <c r="DZ4" s="73"/>
+      <c r="EA4" s="73"/>
+      <c r="EB4" s="73"/>
+      <c r="EC4" s="74"/>
+      <c r="ED4" s="72">
         <f>ED5</f>
         <v>43864</v>
       </c>
-      <c r="EE4" s="74"/>
-      <c r="EF4" s="74"/>
-      <c r="EG4" s="74"/>
-      <c r="EH4" s="74"/>
-      <c r="EI4" s="74"/>
-      <c r="EJ4" s="75"/>
-      <c r="EK4" s="73">
+      <c r="EE4" s="73"/>
+      <c r="EF4" s="73"/>
+      <c r="EG4" s="73"/>
+      <c r="EH4" s="73"/>
+      <c r="EI4" s="73"/>
+      <c r="EJ4" s="74"/>
+      <c r="EK4" s="72">
         <f>EK5</f>
         <v>43871</v>
       </c>
-      <c r="EL4" s="74"/>
-      <c r="EM4" s="74"/>
-      <c r="EN4" s="74"/>
-      <c r="EO4" s="74"/>
-      <c r="EP4" s="74"/>
-      <c r="EQ4" s="75"/>
-      <c r="ER4" s="73">
+      <c r="EL4" s="73"/>
+      <c r="EM4" s="73"/>
+      <c r="EN4" s="73"/>
+      <c r="EO4" s="73"/>
+      <c r="EP4" s="73"/>
+      <c r="EQ4" s="74"/>
+      <c r="ER4" s="72">
         <f>ER5</f>
         <v>43878</v>
       </c>
-      <c r="ES4" s="74"/>
-      <c r="ET4" s="74"/>
-      <c r="EU4" s="74"/>
-      <c r="EV4" s="74"/>
-      <c r="EW4" s="74"/>
-      <c r="EX4" s="75"/>
-      <c r="EY4" s="73">
+      <c r="ES4" s="73"/>
+      <c r="ET4" s="73"/>
+      <c r="EU4" s="73"/>
+      <c r="EV4" s="73"/>
+      <c r="EW4" s="73"/>
+      <c r="EX4" s="74"/>
+      <c r="EY4" s="72">
         <f>EY5</f>
         <v>43885</v>
       </c>
-      <c r="EZ4" s="74"/>
-      <c r="FA4" s="74"/>
-      <c r="FB4" s="74"/>
-      <c r="FC4" s="74"/>
-      <c r="FD4" s="74"/>
-      <c r="FE4" s="75"/>
-      <c r="FF4" s="73">
+      <c r="EZ4" s="73"/>
+      <c r="FA4" s="73"/>
+      <c r="FB4" s="73"/>
+      <c r="FC4" s="73"/>
+      <c r="FD4" s="73"/>
+      <c r="FE4" s="74"/>
+      <c r="FF4" s="72">
         <f>FF5</f>
         <v>43892</v>
       </c>
-      <c r="FG4" s="74"/>
-      <c r="FH4" s="74"/>
-      <c r="FI4" s="74"/>
-      <c r="FJ4" s="74"/>
-      <c r="FK4" s="74"/>
-      <c r="FL4" s="75"/>
-      <c r="FM4" s="73">
+      <c r="FG4" s="73"/>
+      <c r="FH4" s="73"/>
+      <c r="FI4" s="73"/>
+      <c r="FJ4" s="73"/>
+      <c r="FK4" s="73"/>
+      <c r="FL4" s="74"/>
+      <c r="FM4" s="72">
         <f>FM5</f>
         <v>43899</v>
       </c>
-      <c r="FN4" s="74"/>
-      <c r="FO4" s="74"/>
-      <c r="FP4" s="74"/>
-      <c r="FQ4" s="74"/>
-      <c r="FR4" s="74"/>
-      <c r="FS4" s="75"/>
-      <c r="FT4" s="73">
+      <c r="FN4" s="73"/>
+      <c r="FO4" s="73"/>
+      <c r="FP4" s="73"/>
+      <c r="FQ4" s="73"/>
+      <c r="FR4" s="73"/>
+      <c r="FS4" s="74"/>
+      <c r="FT4" s="72">
         <f>FT5</f>
         <v>43906</v>
       </c>
-      <c r="FU4" s="74"/>
-      <c r="FV4" s="74"/>
-      <c r="FW4" s="74"/>
-      <c r="FX4" s="74"/>
-      <c r="FY4" s="74"/>
-      <c r="FZ4" s="75"/>
-      <c r="GA4" s="73">
+      <c r="FU4" s="73"/>
+      <c r="FV4" s="73"/>
+      <c r="FW4" s="73"/>
+      <c r="FX4" s="73"/>
+      <c r="FY4" s="73"/>
+      <c r="FZ4" s="74"/>
+      <c r="GA4" s="72">
         <f>GA5</f>
         <v>43913</v>
       </c>
-      <c r="GB4" s="74"/>
-      <c r="GC4" s="74"/>
-      <c r="GD4" s="74"/>
-      <c r="GE4" s="74"/>
-      <c r="GF4" s="74"/>
-      <c r="GG4" s="75"/>
-      <c r="GH4" s="73">
+      <c r="GB4" s="73"/>
+      <c r="GC4" s="73"/>
+      <c r="GD4" s="73"/>
+      <c r="GE4" s="73"/>
+      <c r="GF4" s="73"/>
+      <c r="GG4" s="74"/>
+      <c r="GH4" s="72">
         <f>GH5</f>
         <v>43920</v>
       </c>
-      <c r="GI4" s="74"/>
-      <c r="GJ4" s="74"/>
-      <c r="GK4" s="74"/>
-      <c r="GL4" s="74"/>
-      <c r="GM4" s="74"/>
-      <c r="GN4" s="75"/>
-      <c r="GO4" s="73">
+      <c r="GI4" s="73"/>
+      <c r="GJ4" s="73"/>
+      <c r="GK4" s="73"/>
+      <c r="GL4" s="73"/>
+      <c r="GM4" s="73"/>
+      <c r="GN4" s="74"/>
+      <c r="GO4" s="72">
         <f>GO5</f>
         <v>43927</v>
       </c>
-      <c r="GP4" s="74"/>
-      <c r="GQ4" s="74"/>
-      <c r="GR4" s="74"/>
-      <c r="GS4" s="74"/>
-      <c r="GT4" s="74"/>
-      <c r="GU4" s="75"/>
+      <c r="GP4" s="73"/>
+      <c r="GQ4" s="73"/>
+      <c r="GR4" s="73"/>
+      <c r="GS4" s="73"/>
+      <c r="GT4" s="73"/>
+      <c r="GU4" s="74"/>
     </row>
     <row r="5" spans="1:203" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
       <c r="H5" s="56">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43738</v>
@@ -4013,7 +4019,7 @@
       <c r="E8" s="42"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11" t="str">
-        <f t="shared" ref="G8:G29" si="109">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="G8:G31" si="109">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="H8" s="18"/>
@@ -4218,10 +4224,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="69" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C9" s="60">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D9" s="43">
         <f>Project_Start</f>
@@ -4654,14 +4660,16 @@
     <row r="11" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="31"/>
       <c r="B11" s="69" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C11" s="60">
-        <v>0.7</v>
-      </c>
-      <c r="D11" s="43"/>
+        <v>1</v>
+      </c>
+      <c r="D11" s="43">
+        <v>43762</v>
+      </c>
       <c r="E11" s="43">
-        <v>43782</v>
+        <v>43783</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
@@ -5079,7 +5087,9 @@
       <c r="B13" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="62"/>
+      <c r="C13" s="62">
+        <v>1</v>
+      </c>
       <c r="D13" s="46">
         <f>E9+1</f>
         <v>43759</v>
@@ -5295,9 +5305,11 @@
       <c r="B14" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="62"/>
+      <c r="C14" s="62">
+        <v>0.3</v>
+      </c>
       <c r="D14" s="46">
-        <f t="shared" ref="D14:D15" si="110">E13+1</f>
+        <f t="shared" ref="D14" si="110">E13+1</f>
         <v>43774</v>
       </c>
       <c r="E14" s="46">
@@ -5509,22 +5521,21 @@
     <row r="15" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="30"/>
       <c r="B15" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="62"/>
+        <v>57</v>
+      </c>
+      <c r="C15" s="62">
+        <v>0</v>
+      </c>
       <c r="D15" s="46">
-        <f t="shared" si="110"/>
+        <f>E14+1</f>
         <v>43789</v>
       </c>
       <c r="E15" s="46">
-        <f>D15+14</f>
-        <v>43803</v>
+        <f>D15+5</f>
+        <v>43794</v>
       </c>
       <c r="F15" s="11"/>
-      <c r="G15" s="11">
-        <f t="shared" si="109"/>
-        <v>15</v>
-      </c>
+      <c r="G15" s="11"/>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
@@ -5537,8 +5548,8 @@
       <c r="Q15" s="18"/>
       <c r="R15" s="18"/>
       <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="18"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="19"/>
       <c r="V15" s="18"/>
       <c r="W15" s="18"/>
       <c r="X15" s="18"/>
@@ -5723,19 +5734,25 @@
       <c r="GU15" s="18"/>
     </row>
     <row r="16" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="63"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="48"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="70" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="62">
+        <v>0</v>
+      </c>
+      <c r="D16" s="46">
+        <f>E15+1</f>
+        <v>43795</v>
+      </c>
+      <c r="E16" s="46">
+        <f>D16+14</f>
+        <v>43809</v>
+      </c>
       <c r="F16" s="11"/>
-      <c r="G16" s="11" t="str">
+      <c r="G16" s="11">
         <f t="shared" si="109"/>
-        <v/>
+        <v>15</v>
       </c>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
@@ -5936,17 +5953,22 @@
     </row>
     <row r="17" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="30"/>
-      <c r="B17" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="64"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
+      <c r="B17" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="62">
+        <v>0</v>
+      </c>
+      <c r="D17" s="46">
+        <f>E16+1</f>
+        <v>43810</v>
+      </c>
+      <c r="E17" s="46">
+        <f>D17+10</f>
+        <v>43820</v>
+      </c>
       <c r="F17" s="11"/>
-      <c r="G17" s="11" t="str">
-        <f t="shared" si="109"/>
-        <v/>
-      </c>
+      <c r="G17" s="11"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
@@ -6145,13 +6167,15 @@
       <c r="GU17" s="18"/>
     </row>
     <row r="18" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="30"/>
-      <c r="B18" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="64"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
+      <c r="A18" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="63"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="48"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11" t="str">
         <f t="shared" si="109"/>
@@ -6357,15 +6381,23 @@
     <row r="19" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30"/>
       <c r="B19" s="71" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="64"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
+        <v>49</v>
+      </c>
+      <c r="C19" s="64">
+        <v>0</v>
+      </c>
+      <c r="D19" s="49">
+        <f>E17+10</f>
+        <v>43830</v>
+      </c>
+      <c r="E19" s="49">
+        <f>D19+10</f>
+        <v>43840</v>
+      </c>
       <c r="F19" s="11"/>
-      <c r="G19" s="11" t="str">
+      <c r="G19" s="11">
         <f t="shared" si="109"/>
-        <v/>
+        <v>11</v>
       </c>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
@@ -6567,15 +6599,23 @@
     <row r="20" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="30"/>
       <c r="B20" s="71" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="64"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
+        <v>50</v>
+      </c>
+      <c r="C20" s="64">
+        <v>0</v>
+      </c>
+      <c r="D20" s="49">
+        <f>E19+1</f>
+        <v>43841</v>
+      </c>
+      <c r="E20" s="49">
+        <f>D20+14</f>
+        <v>43855</v>
+      </c>
       <c r="F20" s="11"/>
-      <c r="G20" s="11" t="str">
+      <c r="G20" s="11">
         <f t="shared" si="109"/>
-        <v/>
+        <v>15</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
@@ -6777,15 +6817,23 @@
     <row r="21" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="30"/>
       <c r="B21" s="71" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="64"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
+        <v>51</v>
+      </c>
+      <c r="C21" s="64">
+        <v>0</v>
+      </c>
+      <c r="D21" s="49">
+        <f>E20+1</f>
+        <v>43856</v>
+      </c>
+      <c r="E21" s="49">
+        <f>D21+1</f>
+        <v>43857</v>
+      </c>
       <c r="F21" s="11"/>
-      <c r="G21" s="11" t="str">
+      <c r="G21" s="11">
         <f t="shared" si="109"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
@@ -6985,19 +7033,25 @@
       <c r="GU21" s="18"/>
     </row>
     <row r="22" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="65"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="51"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="64">
+        <v>0</v>
+      </c>
+      <c r="D22" s="49">
+        <f>E21+1</f>
+        <v>43858</v>
+      </c>
+      <c r="E22" s="49">
+        <f>D22+14</f>
+        <v>43872</v>
+      </c>
       <c r="F22" s="11"/>
-      <c r="G22" s="11" t="str">
+      <c r="G22" s="11">
         <f t="shared" si="109"/>
-        <v/>
+        <v>15</v>
       </c>
       <c r="H22" s="18"/>
       <c r="I22" s="18"/>
@@ -7198,16 +7252,24 @@
     </row>
     <row r="23" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="30"/>
-      <c r="B23" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="66"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
+      <c r="B23" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="64">
+        <v>0</v>
+      </c>
+      <c r="D23" s="49">
+        <f>E22+1</f>
+        <v>43873</v>
+      </c>
+      <c r="E23" s="49">
+        <f>D23+10</f>
+        <v>43883</v>
+      </c>
       <c r="F23" s="11"/>
-      <c r="G23" s="11" t="str">
+      <c r="G23" s="11">
         <f t="shared" si="109"/>
-        <v/>
+        <v>11</v>
       </c>
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
@@ -7407,13 +7469,15 @@
       <c r="GU23" s="18"/>
     </row>
     <row r="24" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="30"/>
-      <c r="B24" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="66"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
+      <c r="A24" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="65"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="51"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11" t="str">
         <f t="shared" si="109"/>
@@ -7619,7 +7683,7 @@
     <row r="25" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="30"/>
       <c r="B25" s="37" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C25" s="66"/>
       <c r="D25" s="52"/>
@@ -7829,7 +7893,7 @@
     <row r="26" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="30"/>
       <c r="B26" s="37" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C26" s="66"/>
       <c r="D26" s="52"/>
@@ -8039,7 +8103,7 @@
     <row r="27" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="30"/>
       <c r="B27" s="37" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C27" s="66"/>
       <c r="D27" s="52"/>
@@ -8247,13 +8311,13 @@
       <c r="GU27" s="18"/>
     </row>
     <row r="28" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="66"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="52"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11" t="str">
         <f t="shared" si="109"/>
@@ -8457,257 +8521,677 @@
       <c r="GU28" s="18"/>
     </row>
     <row r="29" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="68"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17" t="str">
+      <c r="A29" s="30"/>
+      <c r="B29" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="66"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11" t="str">
         <f t="shared" si="109"/>
         <v/>
       </c>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
-      <c r="O29" s="20"/>
-      <c r="P29" s="20"/>
-      <c r="Q29" s="20"/>
-      <c r="R29" s="20"/>
-      <c r="S29" s="20"/>
-      <c r="T29" s="20"/>
-      <c r="U29" s="20"/>
-      <c r="V29" s="20"/>
-      <c r="W29" s="20"/>
-      <c r="X29" s="20"/>
-      <c r="Y29" s="20"/>
-      <c r="Z29" s="20"/>
-      <c r="AA29" s="20"/>
-      <c r="AB29" s="20"/>
-      <c r="AC29" s="20"/>
-      <c r="AD29" s="20"/>
-      <c r="AE29" s="20"/>
-      <c r="AF29" s="20"/>
-      <c r="AG29" s="20"/>
-      <c r="AH29" s="20"/>
-      <c r="AI29" s="20"/>
-      <c r="AJ29" s="20"/>
-      <c r="AK29" s="20"/>
-      <c r="AL29" s="20"/>
-      <c r="AM29" s="20"/>
-      <c r="AN29" s="20"/>
-      <c r="AO29" s="20"/>
-      <c r="AP29" s="20"/>
-      <c r="AQ29" s="20"/>
-      <c r="AR29" s="20"/>
-      <c r="AS29" s="20"/>
-      <c r="AT29" s="20"/>
-      <c r="AU29" s="20"/>
-      <c r="AV29" s="20"/>
-      <c r="AW29" s="20"/>
-      <c r="AX29" s="20"/>
-      <c r="AY29" s="20"/>
-      <c r="AZ29" s="20"/>
-      <c r="BA29" s="20"/>
-      <c r="BB29" s="20"/>
-      <c r="BC29" s="20"/>
-      <c r="BD29" s="20"/>
-      <c r="BE29" s="20"/>
-      <c r="BF29" s="20"/>
-      <c r="BG29" s="20"/>
-      <c r="BH29" s="20"/>
-      <c r="BI29" s="20"/>
-      <c r="BJ29" s="20"/>
-      <c r="BK29" s="20"/>
-      <c r="BL29" s="20"/>
-      <c r="BM29" s="20"/>
-      <c r="BN29" s="20"/>
-      <c r="BO29" s="20"/>
-      <c r="BP29" s="20"/>
-      <c r="BQ29" s="20"/>
-      <c r="BR29" s="20"/>
-      <c r="BS29" s="20"/>
-      <c r="BT29" s="20"/>
-      <c r="BU29" s="20"/>
-      <c r="BV29" s="20"/>
-      <c r="BW29" s="20"/>
-      <c r="BX29" s="20"/>
-      <c r="BY29" s="20"/>
-      <c r="BZ29" s="20"/>
-      <c r="CA29" s="20"/>
-      <c r="CB29" s="20"/>
-      <c r="CC29" s="20"/>
-      <c r="CD29" s="20"/>
-      <c r="CE29" s="20"/>
-      <c r="CF29" s="20"/>
-      <c r="CG29" s="20"/>
-      <c r="CH29" s="20"/>
-      <c r="CI29" s="20"/>
-      <c r="CJ29" s="20"/>
-      <c r="CK29" s="20"/>
-      <c r="CL29" s="20"/>
-      <c r="CM29" s="20"/>
-      <c r="CN29" s="20"/>
-      <c r="CO29" s="20"/>
-      <c r="CP29" s="20"/>
-      <c r="CQ29" s="20"/>
-      <c r="CR29" s="20"/>
-      <c r="CS29" s="20"/>
-      <c r="CT29" s="20"/>
-      <c r="CU29" s="20"/>
-      <c r="CV29" s="20"/>
-      <c r="CW29" s="20"/>
-      <c r="CX29" s="20"/>
-      <c r="CY29" s="20"/>
-      <c r="CZ29" s="20"/>
-      <c r="DA29" s="20"/>
-      <c r="DB29" s="20"/>
-      <c r="DC29" s="20"/>
-      <c r="DD29" s="20"/>
-      <c r="DE29" s="20"/>
-      <c r="DF29" s="20"/>
-      <c r="DG29" s="20"/>
-      <c r="DH29" s="20"/>
-      <c r="DI29" s="20"/>
-      <c r="DJ29" s="20"/>
-      <c r="DK29" s="20"/>
-      <c r="DL29" s="20"/>
-      <c r="DM29" s="20"/>
-      <c r="DN29" s="20"/>
-      <c r="DO29" s="20"/>
-      <c r="DP29" s="20"/>
-      <c r="DQ29" s="20"/>
-      <c r="DR29" s="20"/>
-      <c r="DS29" s="20"/>
-      <c r="DT29" s="20"/>
-      <c r="DU29" s="20"/>
-      <c r="DV29" s="20"/>
-      <c r="DW29" s="20"/>
-      <c r="DX29" s="20"/>
-      <c r="DY29" s="20"/>
-      <c r="DZ29" s="20"/>
-      <c r="EA29" s="20"/>
-      <c r="EB29" s="20"/>
-      <c r="EC29" s="20"/>
-      <c r="ED29" s="20"/>
-      <c r="EE29" s="20"/>
-      <c r="EF29" s="20"/>
-      <c r="EG29" s="20"/>
-      <c r="EH29" s="20"/>
-      <c r="EI29" s="20"/>
-      <c r="EJ29" s="20"/>
-      <c r="EK29" s="20"/>
-      <c r="EL29" s="20"/>
-      <c r="EM29" s="20"/>
-      <c r="EN29" s="20"/>
-      <c r="EO29" s="20"/>
-      <c r="EP29" s="20"/>
-      <c r="EQ29" s="20"/>
-      <c r="ER29" s="20"/>
-      <c r="ES29" s="20"/>
-      <c r="ET29" s="20"/>
-      <c r="EU29" s="20"/>
-      <c r="EV29" s="20"/>
-      <c r="EW29" s="20"/>
-      <c r="EX29" s="20"/>
-      <c r="EY29" s="20"/>
-      <c r="EZ29" s="20"/>
-      <c r="FA29" s="20"/>
-      <c r="FB29" s="20"/>
-      <c r="FC29" s="20"/>
-      <c r="FD29" s="20"/>
-      <c r="FE29" s="20"/>
-      <c r="FF29" s="20"/>
-      <c r="FG29" s="20"/>
-      <c r="FH29" s="20"/>
-      <c r="FI29" s="20"/>
-      <c r="FJ29" s="20"/>
-      <c r="FK29" s="20"/>
-      <c r="FL29" s="20"/>
-      <c r="FM29" s="20"/>
-      <c r="FN29" s="20"/>
-      <c r="FO29" s="20"/>
-      <c r="FP29" s="20"/>
-      <c r="FQ29" s="20"/>
-      <c r="FR29" s="20"/>
-      <c r="FS29" s="20"/>
-      <c r="FT29" s="20"/>
-      <c r="FU29" s="20"/>
-      <c r="FV29" s="20"/>
-      <c r="FW29" s="20"/>
-      <c r="FX29" s="20"/>
-      <c r="FY29" s="20"/>
-      <c r="FZ29" s="20"/>
-      <c r="GA29" s="20"/>
-      <c r="GB29" s="20"/>
-      <c r="GC29" s="20"/>
-      <c r="GD29" s="20"/>
-      <c r="GE29" s="20"/>
-      <c r="GF29" s="20"/>
-      <c r="GG29" s="20"/>
-      <c r="GH29" s="20"/>
-      <c r="GI29" s="20"/>
-      <c r="GJ29" s="20"/>
-      <c r="GK29" s="20"/>
-      <c r="GL29" s="20"/>
-      <c r="GM29" s="20"/>
-      <c r="GN29" s="20"/>
-      <c r="GO29" s="20"/>
-      <c r="GP29" s="20"/>
-      <c r="GQ29" s="20"/>
-      <c r="GR29" s="20"/>
-      <c r="GS29" s="20"/>
-      <c r="GT29" s="20"/>
-      <c r="GU29" s="20"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="18"/>
+      <c r="S29" s="18"/>
+      <c r="T29" s="18"/>
+      <c r="U29" s="18"/>
+      <c r="V29" s="18"/>
+      <c r="W29" s="18"/>
+      <c r="X29" s="18"/>
+      <c r="Y29" s="18"/>
+      <c r="Z29" s="18"/>
+      <c r="AA29" s="18"/>
+      <c r="AB29" s="18"/>
+      <c r="AC29" s="18"/>
+      <c r="AD29" s="18"/>
+      <c r="AE29" s="18"/>
+      <c r="AF29" s="18"/>
+      <c r="AG29" s="18"/>
+      <c r="AH29" s="18"/>
+      <c r="AI29" s="18"/>
+      <c r="AJ29" s="18"/>
+      <c r="AK29" s="18"/>
+      <c r="AL29" s="18"/>
+      <c r="AM29" s="18"/>
+      <c r="AN29" s="18"/>
+      <c r="AO29" s="18"/>
+      <c r="AP29" s="18"/>
+      <c r="AQ29" s="18"/>
+      <c r="AR29" s="18"/>
+      <c r="AS29" s="18"/>
+      <c r="AT29" s="18"/>
+      <c r="AU29" s="18"/>
+      <c r="AV29" s="18"/>
+      <c r="AW29" s="18"/>
+      <c r="AX29" s="18"/>
+      <c r="AY29" s="18"/>
+      <c r="AZ29" s="18"/>
+      <c r="BA29" s="18"/>
+      <c r="BB29" s="18"/>
+      <c r="BC29" s="18"/>
+      <c r="BD29" s="18"/>
+      <c r="BE29" s="18"/>
+      <c r="BF29" s="18"/>
+      <c r="BG29" s="18"/>
+      <c r="BH29" s="18"/>
+      <c r="BI29" s="18"/>
+      <c r="BJ29" s="18"/>
+      <c r="BK29" s="18"/>
+      <c r="BL29" s="18"/>
+      <c r="BM29" s="18"/>
+      <c r="BN29" s="18"/>
+      <c r="BO29" s="18"/>
+      <c r="BP29" s="18"/>
+      <c r="BQ29" s="18"/>
+      <c r="BR29" s="18"/>
+      <c r="BS29" s="18"/>
+      <c r="BT29" s="18"/>
+      <c r="BU29" s="18"/>
+      <c r="BV29" s="18"/>
+      <c r="BW29" s="18"/>
+      <c r="BX29" s="18"/>
+      <c r="BY29" s="18"/>
+      <c r="BZ29" s="18"/>
+      <c r="CA29" s="18"/>
+      <c r="CB29" s="18"/>
+      <c r="CC29" s="18"/>
+      <c r="CD29" s="18"/>
+      <c r="CE29" s="18"/>
+      <c r="CF29" s="18"/>
+      <c r="CG29" s="18"/>
+      <c r="CH29" s="18"/>
+      <c r="CI29" s="18"/>
+      <c r="CJ29" s="18"/>
+      <c r="CK29" s="18"/>
+      <c r="CL29" s="18"/>
+      <c r="CM29" s="18"/>
+      <c r="CN29" s="18"/>
+      <c r="CO29" s="18"/>
+      <c r="CP29" s="18"/>
+      <c r="CQ29" s="18"/>
+      <c r="CR29" s="18"/>
+      <c r="CS29" s="18"/>
+      <c r="CT29" s="18"/>
+      <c r="CU29" s="18"/>
+      <c r="CV29" s="18"/>
+      <c r="CW29" s="18"/>
+      <c r="CX29" s="18"/>
+      <c r="CY29" s="18"/>
+      <c r="CZ29" s="18"/>
+      <c r="DA29" s="18"/>
+      <c r="DB29" s="18"/>
+      <c r="DC29" s="18"/>
+      <c r="DD29" s="18"/>
+      <c r="DE29" s="18"/>
+      <c r="DF29" s="18"/>
+      <c r="DG29" s="18"/>
+      <c r="DH29" s="18"/>
+      <c r="DI29" s="18"/>
+      <c r="DJ29" s="18"/>
+      <c r="DK29" s="18"/>
+      <c r="DL29" s="18"/>
+      <c r="DM29" s="18"/>
+      <c r="DN29" s="18"/>
+      <c r="DO29" s="18"/>
+      <c r="DP29" s="18"/>
+      <c r="DQ29" s="18"/>
+      <c r="DR29" s="18"/>
+      <c r="DS29" s="18"/>
+      <c r="DT29" s="18"/>
+      <c r="DU29" s="18"/>
+      <c r="DV29" s="18"/>
+      <c r="DW29" s="18"/>
+      <c r="DX29" s="18"/>
+      <c r="DY29" s="18"/>
+      <c r="DZ29" s="18"/>
+      <c r="EA29" s="18"/>
+      <c r="EB29" s="18"/>
+      <c r="EC29" s="18"/>
+      <c r="ED29" s="18"/>
+      <c r="EE29" s="18"/>
+      <c r="EF29" s="18"/>
+      <c r="EG29" s="18"/>
+      <c r="EH29" s="18"/>
+      <c r="EI29" s="18"/>
+      <c r="EJ29" s="18"/>
+      <c r="EK29" s="18"/>
+      <c r="EL29" s="18"/>
+      <c r="EM29" s="18"/>
+      <c r="EN29" s="18"/>
+      <c r="EO29" s="18"/>
+      <c r="EP29" s="18"/>
+      <c r="EQ29" s="18"/>
+      <c r="ER29" s="18"/>
+      <c r="ES29" s="18"/>
+      <c r="ET29" s="18"/>
+      <c r="EU29" s="18"/>
+      <c r="EV29" s="18"/>
+      <c r="EW29" s="18"/>
+      <c r="EX29" s="18"/>
+      <c r="EY29" s="18"/>
+      <c r="EZ29" s="18"/>
+      <c r="FA29" s="18"/>
+      <c r="FB29" s="18"/>
+      <c r="FC29" s="18"/>
+      <c r="FD29" s="18"/>
+      <c r="FE29" s="18"/>
+      <c r="FF29" s="18"/>
+      <c r="FG29" s="18"/>
+      <c r="FH29" s="18"/>
+      <c r="FI29" s="18"/>
+      <c r="FJ29" s="18"/>
+      <c r="FK29" s="18"/>
+      <c r="FL29" s="18"/>
+      <c r="FM29" s="18"/>
+      <c r="FN29" s="18"/>
+      <c r="FO29" s="18"/>
+      <c r="FP29" s="18"/>
+      <c r="FQ29" s="18"/>
+      <c r="FR29" s="18"/>
+      <c r="FS29" s="18"/>
+      <c r="FT29" s="18"/>
+      <c r="FU29" s="18"/>
+      <c r="FV29" s="18"/>
+      <c r="FW29" s="18"/>
+      <c r="FX29" s="18"/>
+      <c r="FY29" s="18"/>
+      <c r="FZ29" s="18"/>
+      <c r="GA29" s="18"/>
+      <c r="GB29" s="18"/>
+      <c r="GC29" s="18"/>
+      <c r="GD29" s="18"/>
+      <c r="GE29" s="18"/>
+      <c r="GF29" s="18"/>
+      <c r="GG29" s="18"/>
+      <c r="GH29" s="18"/>
+      <c r="GI29" s="18"/>
+      <c r="GJ29" s="18"/>
+      <c r="GK29" s="18"/>
+      <c r="GL29" s="18"/>
+      <c r="GM29" s="18"/>
+      <c r="GN29" s="18"/>
+      <c r="GO29" s="18"/>
+      <c r="GP29" s="18"/>
+      <c r="GQ29" s="18"/>
+      <c r="GR29" s="18"/>
+      <c r="GS29" s="18"/>
+      <c r="GT29" s="18"/>
+      <c r="GU29" s="18"/>
     </row>
-    <row r="30" spans="1:203" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F30" s="5"/>
+    <row r="30" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="38"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11" t="str">
+        <f t="shared" si="109"/>
+        <v/>
+      </c>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18"/>
+      <c r="S30" s="18"/>
+      <c r="T30" s="18"/>
+      <c r="U30" s="18"/>
+      <c r="V30" s="18"/>
+      <c r="W30" s="18"/>
+      <c r="X30" s="18"/>
+      <c r="Y30" s="18"/>
+      <c r="Z30" s="18"/>
+      <c r="AA30" s="18"/>
+      <c r="AB30" s="18"/>
+      <c r="AC30" s="18"/>
+      <c r="AD30" s="18"/>
+      <c r="AE30" s="18"/>
+      <c r="AF30" s="18"/>
+      <c r="AG30" s="18"/>
+      <c r="AH30" s="18"/>
+      <c r="AI30" s="18"/>
+      <c r="AJ30" s="18"/>
+      <c r="AK30" s="18"/>
+      <c r="AL30" s="18"/>
+      <c r="AM30" s="18"/>
+      <c r="AN30" s="18"/>
+      <c r="AO30" s="18"/>
+      <c r="AP30" s="18"/>
+      <c r="AQ30" s="18"/>
+      <c r="AR30" s="18"/>
+      <c r="AS30" s="18"/>
+      <c r="AT30" s="18"/>
+      <c r="AU30" s="18"/>
+      <c r="AV30" s="18"/>
+      <c r="AW30" s="18"/>
+      <c r="AX30" s="18"/>
+      <c r="AY30" s="18"/>
+      <c r="AZ30" s="18"/>
+      <c r="BA30" s="18"/>
+      <c r="BB30" s="18"/>
+      <c r="BC30" s="18"/>
+      <c r="BD30" s="18"/>
+      <c r="BE30" s="18"/>
+      <c r="BF30" s="18"/>
+      <c r="BG30" s="18"/>
+      <c r="BH30" s="18"/>
+      <c r="BI30" s="18"/>
+      <c r="BJ30" s="18"/>
+      <c r="BK30" s="18"/>
+      <c r="BL30" s="18"/>
+      <c r="BM30" s="18"/>
+      <c r="BN30" s="18"/>
+      <c r="BO30" s="18"/>
+      <c r="BP30" s="18"/>
+      <c r="BQ30" s="18"/>
+      <c r="BR30" s="18"/>
+      <c r="BS30" s="18"/>
+      <c r="BT30" s="18"/>
+      <c r="BU30" s="18"/>
+      <c r="BV30" s="18"/>
+      <c r="BW30" s="18"/>
+      <c r="BX30" s="18"/>
+      <c r="BY30" s="18"/>
+      <c r="BZ30" s="18"/>
+      <c r="CA30" s="18"/>
+      <c r="CB30" s="18"/>
+      <c r="CC30" s="18"/>
+      <c r="CD30" s="18"/>
+      <c r="CE30" s="18"/>
+      <c r="CF30" s="18"/>
+      <c r="CG30" s="18"/>
+      <c r="CH30" s="18"/>
+      <c r="CI30" s="18"/>
+      <c r="CJ30" s="18"/>
+      <c r="CK30" s="18"/>
+      <c r="CL30" s="18"/>
+      <c r="CM30" s="18"/>
+      <c r="CN30" s="18"/>
+      <c r="CO30" s="18"/>
+      <c r="CP30" s="18"/>
+      <c r="CQ30" s="18"/>
+      <c r="CR30" s="18"/>
+      <c r="CS30" s="18"/>
+      <c r="CT30" s="18"/>
+      <c r="CU30" s="18"/>
+      <c r="CV30" s="18"/>
+      <c r="CW30" s="18"/>
+      <c r="CX30" s="18"/>
+      <c r="CY30" s="18"/>
+      <c r="CZ30" s="18"/>
+      <c r="DA30" s="18"/>
+      <c r="DB30" s="18"/>
+      <c r="DC30" s="18"/>
+      <c r="DD30" s="18"/>
+      <c r="DE30" s="18"/>
+      <c r="DF30" s="18"/>
+      <c r="DG30" s="18"/>
+      <c r="DH30" s="18"/>
+      <c r="DI30" s="18"/>
+      <c r="DJ30" s="18"/>
+      <c r="DK30" s="18"/>
+      <c r="DL30" s="18"/>
+      <c r="DM30" s="18"/>
+      <c r="DN30" s="18"/>
+      <c r="DO30" s="18"/>
+      <c r="DP30" s="18"/>
+      <c r="DQ30" s="18"/>
+      <c r="DR30" s="18"/>
+      <c r="DS30" s="18"/>
+      <c r="DT30" s="18"/>
+      <c r="DU30" s="18"/>
+      <c r="DV30" s="18"/>
+      <c r="DW30" s="18"/>
+      <c r="DX30" s="18"/>
+      <c r="DY30" s="18"/>
+      <c r="DZ30" s="18"/>
+      <c r="EA30" s="18"/>
+      <c r="EB30" s="18"/>
+      <c r="EC30" s="18"/>
+      <c r="ED30" s="18"/>
+      <c r="EE30" s="18"/>
+      <c r="EF30" s="18"/>
+      <c r="EG30" s="18"/>
+      <c r="EH30" s="18"/>
+      <c r="EI30" s="18"/>
+      <c r="EJ30" s="18"/>
+      <c r="EK30" s="18"/>
+      <c r="EL30" s="18"/>
+      <c r="EM30" s="18"/>
+      <c r="EN30" s="18"/>
+      <c r="EO30" s="18"/>
+      <c r="EP30" s="18"/>
+      <c r="EQ30" s="18"/>
+      <c r="ER30" s="18"/>
+      <c r="ES30" s="18"/>
+      <c r="ET30" s="18"/>
+      <c r="EU30" s="18"/>
+      <c r="EV30" s="18"/>
+      <c r="EW30" s="18"/>
+      <c r="EX30" s="18"/>
+      <c r="EY30" s="18"/>
+      <c r="EZ30" s="18"/>
+      <c r="FA30" s="18"/>
+      <c r="FB30" s="18"/>
+      <c r="FC30" s="18"/>
+      <c r="FD30" s="18"/>
+      <c r="FE30" s="18"/>
+      <c r="FF30" s="18"/>
+      <c r="FG30" s="18"/>
+      <c r="FH30" s="18"/>
+      <c r="FI30" s="18"/>
+      <c r="FJ30" s="18"/>
+      <c r="FK30" s="18"/>
+      <c r="FL30" s="18"/>
+      <c r="FM30" s="18"/>
+      <c r="FN30" s="18"/>
+      <c r="FO30" s="18"/>
+      <c r="FP30" s="18"/>
+      <c r="FQ30" s="18"/>
+      <c r="FR30" s="18"/>
+      <c r="FS30" s="18"/>
+      <c r="FT30" s="18"/>
+      <c r="FU30" s="18"/>
+      <c r="FV30" s="18"/>
+      <c r="FW30" s="18"/>
+      <c r="FX30" s="18"/>
+      <c r="FY30" s="18"/>
+      <c r="FZ30" s="18"/>
+      <c r="GA30" s="18"/>
+      <c r="GB30" s="18"/>
+      <c r="GC30" s="18"/>
+      <c r="GD30" s="18"/>
+      <c r="GE30" s="18"/>
+      <c r="GF30" s="18"/>
+      <c r="GG30" s="18"/>
+      <c r="GH30" s="18"/>
+      <c r="GI30" s="18"/>
+      <c r="GJ30" s="18"/>
+      <c r="GK30" s="18"/>
+      <c r="GL30" s="18"/>
+      <c r="GM30" s="18"/>
+      <c r="GN30" s="18"/>
+      <c r="GO30" s="18"/>
+      <c r="GP30" s="18"/>
+      <c r="GQ30" s="18"/>
+      <c r="GR30" s="18"/>
+      <c r="GS30" s="18"/>
+      <c r="GT30" s="18"/>
+      <c r="GU30" s="18"/>
     </row>
-    <row r="31" spans="1:203" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E31" s="32"/>
+    <row r="31" spans="1:203" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="68"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17" t="str">
+        <f t="shared" si="109"/>
+        <v/>
+      </c>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
+      <c r="O31" s="20"/>
+      <c r="P31" s="20"/>
+      <c r="Q31" s="20"/>
+      <c r="R31" s="20"/>
+      <c r="S31" s="20"/>
+      <c r="T31" s="20"/>
+      <c r="U31" s="20"/>
+      <c r="V31" s="20"/>
+      <c r="W31" s="20"/>
+      <c r="X31" s="20"/>
+      <c r="Y31" s="20"/>
+      <c r="Z31" s="20"/>
+      <c r="AA31" s="20"/>
+      <c r="AB31" s="20"/>
+      <c r="AC31" s="20"/>
+      <c r="AD31" s="20"/>
+      <c r="AE31" s="20"/>
+      <c r="AF31" s="20"/>
+      <c r="AG31" s="20"/>
+      <c r="AH31" s="20"/>
+      <c r="AI31" s="20"/>
+      <c r="AJ31" s="20"/>
+      <c r="AK31" s="20"/>
+      <c r="AL31" s="20"/>
+      <c r="AM31" s="20"/>
+      <c r="AN31" s="20"/>
+      <c r="AO31" s="20"/>
+      <c r="AP31" s="20"/>
+      <c r="AQ31" s="20"/>
+      <c r="AR31" s="20"/>
+      <c r="AS31" s="20"/>
+      <c r="AT31" s="20"/>
+      <c r="AU31" s="20"/>
+      <c r="AV31" s="20"/>
+      <c r="AW31" s="20"/>
+      <c r="AX31" s="20"/>
+      <c r="AY31" s="20"/>
+      <c r="AZ31" s="20"/>
+      <c r="BA31" s="20"/>
+      <c r="BB31" s="20"/>
+      <c r="BC31" s="20"/>
+      <c r="BD31" s="20"/>
+      <c r="BE31" s="20"/>
+      <c r="BF31" s="20"/>
+      <c r="BG31" s="20"/>
+      <c r="BH31" s="20"/>
+      <c r="BI31" s="20"/>
+      <c r="BJ31" s="20"/>
+      <c r="BK31" s="20"/>
+      <c r="BL31" s="20"/>
+      <c r="BM31" s="20"/>
+      <c r="BN31" s="20"/>
+      <c r="BO31" s="20"/>
+      <c r="BP31" s="20"/>
+      <c r="BQ31" s="20"/>
+      <c r="BR31" s="20"/>
+      <c r="BS31" s="20"/>
+      <c r="BT31" s="20"/>
+      <c r="BU31" s="20"/>
+      <c r="BV31" s="20"/>
+      <c r="BW31" s="20"/>
+      <c r="BX31" s="20"/>
+      <c r="BY31" s="20"/>
+      <c r="BZ31" s="20"/>
+      <c r="CA31" s="20"/>
+      <c r="CB31" s="20"/>
+      <c r="CC31" s="20"/>
+      <c r="CD31" s="20"/>
+      <c r="CE31" s="20"/>
+      <c r="CF31" s="20"/>
+      <c r="CG31" s="20"/>
+      <c r="CH31" s="20"/>
+      <c r="CI31" s="20"/>
+      <c r="CJ31" s="20"/>
+      <c r="CK31" s="20"/>
+      <c r="CL31" s="20"/>
+      <c r="CM31" s="20"/>
+      <c r="CN31" s="20"/>
+      <c r="CO31" s="20"/>
+      <c r="CP31" s="20"/>
+      <c r="CQ31" s="20"/>
+      <c r="CR31" s="20"/>
+      <c r="CS31" s="20"/>
+      <c r="CT31" s="20"/>
+      <c r="CU31" s="20"/>
+      <c r="CV31" s="20"/>
+      <c r="CW31" s="20"/>
+      <c r="CX31" s="20"/>
+      <c r="CY31" s="20"/>
+      <c r="CZ31" s="20"/>
+      <c r="DA31" s="20"/>
+      <c r="DB31" s="20"/>
+      <c r="DC31" s="20"/>
+      <c r="DD31" s="20"/>
+      <c r="DE31" s="20"/>
+      <c r="DF31" s="20"/>
+      <c r="DG31" s="20"/>
+      <c r="DH31" s="20"/>
+      <c r="DI31" s="20"/>
+      <c r="DJ31" s="20"/>
+      <c r="DK31" s="20"/>
+      <c r="DL31" s="20"/>
+      <c r="DM31" s="20"/>
+      <c r="DN31" s="20"/>
+      <c r="DO31" s="20"/>
+      <c r="DP31" s="20"/>
+      <c r="DQ31" s="20"/>
+      <c r="DR31" s="20"/>
+      <c r="DS31" s="20"/>
+      <c r="DT31" s="20"/>
+      <c r="DU31" s="20"/>
+      <c r="DV31" s="20"/>
+      <c r="DW31" s="20"/>
+      <c r="DX31" s="20"/>
+      <c r="DY31" s="20"/>
+      <c r="DZ31" s="20"/>
+      <c r="EA31" s="20"/>
+      <c r="EB31" s="20"/>
+      <c r="EC31" s="20"/>
+      <c r="ED31" s="20"/>
+      <c r="EE31" s="20"/>
+      <c r="EF31" s="20"/>
+      <c r="EG31" s="20"/>
+      <c r="EH31" s="20"/>
+      <c r="EI31" s="20"/>
+      <c r="EJ31" s="20"/>
+      <c r="EK31" s="20"/>
+      <c r="EL31" s="20"/>
+      <c r="EM31" s="20"/>
+      <c r="EN31" s="20"/>
+      <c r="EO31" s="20"/>
+      <c r="EP31" s="20"/>
+      <c r="EQ31" s="20"/>
+      <c r="ER31" s="20"/>
+      <c r="ES31" s="20"/>
+      <c r="ET31" s="20"/>
+      <c r="EU31" s="20"/>
+      <c r="EV31" s="20"/>
+      <c r="EW31" s="20"/>
+      <c r="EX31" s="20"/>
+      <c r="EY31" s="20"/>
+      <c r="EZ31" s="20"/>
+      <c r="FA31" s="20"/>
+      <c r="FB31" s="20"/>
+      <c r="FC31" s="20"/>
+      <c r="FD31" s="20"/>
+      <c r="FE31" s="20"/>
+      <c r="FF31" s="20"/>
+      <c r="FG31" s="20"/>
+      <c r="FH31" s="20"/>
+      <c r="FI31" s="20"/>
+      <c r="FJ31" s="20"/>
+      <c r="FK31" s="20"/>
+      <c r="FL31" s="20"/>
+      <c r="FM31" s="20"/>
+      <c r="FN31" s="20"/>
+      <c r="FO31" s="20"/>
+      <c r="FP31" s="20"/>
+      <c r="FQ31" s="20"/>
+      <c r="FR31" s="20"/>
+      <c r="FS31" s="20"/>
+      <c r="FT31" s="20"/>
+      <c r="FU31" s="20"/>
+      <c r="FV31" s="20"/>
+      <c r="FW31" s="20"/>
+      <c r="FX31" s="20"/>
+      <c r="FY31" s="20"/>
+      <c r="FZ31" s="20"/>
+      <c r="GA31" s="20"/>
+      <c r="GB31" s="20"/>
+      <c r="GC31" s="20"/>
+      <c r="GD31" s="20"/>
+      <c r="GE31" s="20"/>
+      <c r="GF31" s="20"/>
+      <c r="GG31" s="20"/>
+      <c r="GH31" s="20"/>
+      <c r="GI31" s="20"/>
+      <c r="GJ31" s="20"/>
+      <c r="GK31" s="20"/>
+      <c r="GL31" s="20"/>
+      <c r="GM31" s="20"/>
+      <c r="GN31" s="20"/>
+      <c r="GO31" s="20"/>
+      <c r="GP31" s="20"/>
+      <c r="GQ31" s="20"/>
+      <c r="GR31" s="20"/>
+      <c r="GS31" s="20"/>
+      <c r="GT31" s="20"/>
+      <c r="GU31" s="20"/>
+    </row>
+    <row r="32" spans="1:203" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="H4:N4"/>
+    <mergeCell ref="O4:U4"/>
+    <mergeCell ref="V4:AB4"/>
+    <mergeCell ref="AC4:AI4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="AJ4:AP4"/>
+    <mergeCell ref="AQ4:AW4"/>
+    <mergeCell ref="AX4:BD4"/>
+    <mergeCell ref="BE4:BK4"/>
+    <mergeCell ref="BL4:BR4"/>
+    <mergeCell ref="BS4:BY4"/>
+    <mergeCell ref="BZ4:CF4"/>
+    <mergeCell ref="CG4:CM4"/>
+    <mergeCell ref="CN4:CT4"/>
+    <mergeCell ref="CU4:DA4"/>
+    <mergeCell ref="DB4:DH4"/>
+    <mergeCell ref="DI4:DO4"/>
+    <mergeCell ref="DP4:DV4"/>
+    <mergeCell ref="DW4:EC4"/>
+    <mergeCell ref="ED4:EJ4"/>
+    <mergeCell ref="EK4:EQ4"/>
+    <mergeCell ref="ER4:EX4"/>
+    <mergeCell ref="EY4:FE4"/>
+    <mergeCell ref="FF4:FL4"/>
     <mergeCell ref="FM4:FS4"/>
     <mergeCell ref="FT4:FZ4"/>
     <mergeCell ref="GA4:GG4"/>
     <mergeCell ref="GH4:GN4"/>
     <mergeCell ref="GO4:GU4"/>
-    <mergeCell ref="ED4:EJ4"/>
-    <mergeCell ref="EK4:EQ4"/>
-    <mergeCell ref="ER4:EX4"/>
-    <mergeCell ref="EY4:FE4"/>
-    <mergeCell ref="FF4:FL4"/>
-    <mergeCell ref="CU4:DA4"/>
-    <mergeCell ref="DB4:DH4"/>
-    <mergeCell ref="DI4:DO4"/>
-    <mergeCell ref="DP4:DV4"/>
-    <mergeCell ref="DW4:EC4"/>
-    <mergeCell ref="BL4:BR4"/>
-    <mergeCell ref="BS4:BY4"/>
-    <mergeCell ref="BZ4:CF4"/>
-    <mergeCell ref="CG4:CM4"/>
-    <mergeCell ref="CN4:CT4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="AJ4:AP4"/>
-    <mergeCell ref="AQ4:AW4"/>
-    <mergeCell ref="AX4:BD4"/>
-    <mergeCell ref="BE4:BK4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="H4:N4"/>
-    <mergeCell ref="O4:U4"/>
-    <mergeCell ref="V4:AB4"/>
-    <mergeCell ref="AC4:AI4"/>
   </mergeCells>
-  <conditionalFormatting sqref="C7:C29">
+  <conditionalFormatting sqref="C7:C31">
     <cfRule type="dataBar" priority="44">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8721,12 +9205,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:GU29">
+  <conditionalFormatting sqref="H5:GU31">
     <cfRule type="expression" dxfId="2" priority="63">
       <formula>AND(TODAY()&gt;=H$5,TODAY()&lt;I$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:GU29">
+  <conditionalFormatting sqref="H7:GU31">
     <cfRule type="expression" dxfId="1" priority="57">
       <formula>AND(task_start&lt;=H$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=H$5)</formula>
     </cfRule>
@@ -8741,7 +9225,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="60" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="24" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -8761,7 +9245,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>C7:C29</xm:sqref>
+          <xm:sqref>C7:C31</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>